<commit_message>
files for Leipzig presentation.
</commit_message>
<xml_diff>
--- a/Leipzig_Dec15/Polybius_consolidated_files.xlsx
+++ b/Leipzig_Dec15/Polybius_consolidated_files.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="zscores_Oct11" sheetId="1" r:id="rId1"/>
@@ -2567,10 +2567,10 @@
   <dimension ref="A1:AOU25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="GQ4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="CI4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:GS24"/>
+      <selection pane="bottomRight" activeCell="CP2" sqref="CP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63664,13 +63664,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GS24"/>
+  <dimension ref="A1:GS26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69725,608 +69725,608 @@
         <v>1.50285542530809E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:201" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:201" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>-0.52404020966414</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>-0.70100573378826303</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>-0.58244302380061896</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1.0113647790037199</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>1.4762966124911101</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.97349194912708104</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>0.46637120332829501</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>2.1989860803519798</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>1.94776567786431</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <v>-0.67231757454865204</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="2">
         <v>0.25644222229383501</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="2">
         <v>0.63805073449717797</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="2">
         <v>-0.71439375520535697</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="2">
         <v>1.1271267067735999</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="2">
         <v>1.6518108419213799</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
         <v>0.164307871888866</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="2">
         <v>0.375688678433797</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="2">
         <v>1.2558801236744801</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="2">
         <v>0.63657401112282996</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="2">
         <v>0.582941698013968</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="2">
         <v>1.0605630662601699</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="2">
         <v>0.91767731206302094</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="2">
         <v>-0.51617892763371798</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="2">
         <v>1.61089982523577</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="2">
         <v>-4.9220178853857197E-2</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="2">
         <v>2.1408385932918801</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="2">
         <v>1.4900415747334601</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="2">
         <v>0.36746732650203301</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="2">
         <v>0.76366959240275101</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="2">
         <v>-0.118450054141227</v>
       </c>
-      <c r="AF11">
+      <c r="AF11" s="2">
         <v>1.1173524326212301</v>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="2">
         <v>2.1920102953957299</v>
       </c>
-      <c r="AH11">
+      <c r="AH11" s="2">
         <v>-0.40763037077735897</v>
       </c>
-      <c r="AI11">
+      <c r="AI11" s="2">
         <v>-0.58333846407009105</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="2">
         <v>0.38478246951449102</v>
       </c>
-      <c r="AK11">
+      <c r="AK11" s="2">
         <v>2.31329529801565</v>
       </c>
-      <c r="AL11">
+      <c r="AL11" s="2">
         <v>0.48806683964578601</v>
       </c>
-      <c r="AM11">
+      <c r="AM11" s="2">
         <v>0.26946316921340802</v>
       </c>
-      <c r="AN11">
+      <c r="AN11" s="2">
         <v>-0.432576966589379</v>
       </c>
-      <c r="AO11">
+      <c r="AO11" s="2">
         <v>1.8656893503062</v>
       </c>
-      <c r="AP11">
+      <c r="AP11" s="2">
         <v>-7.9321400493697097E-2</v>
       </c>
-      <c r="AQ11">
+      <c r="AQ11" s="2">
         <v>0.54586858579918196</v>
       </c>
-      <c r="AR11">
+      <c r="AR11" s="2">
         <v>0.23999868053526799</v>
       </c>
-      <c r="AS11">
+      <c r="AS11" s="2">
         <v>-0.655397251254077</v>
       </c>
-      <c r="AT11">
+      <c r="AT11" s="2">
         <v>-0.104739339561712</v>
       </c>
-      <c r="AU11">
+      <c r="AU11" s="2">
         <v>0.92173039620334196</v>
       </c>
-      <c r="AV11">
+      <c r="AV11" s="2">
         <v>1.1089181244188</v>
       </c>
-      <c r="AW11">
+      <c r="AW11" s="2">
         <v>-0.79988234490878396</v>
       </c>
-      <c r="AX11">
+      <c r="AX11" s="2">
         <v>-8.3539756518516195E-2</v>
       </c>
-      <c r="AY11">
+      <c r="AY11" s="2">
         <v>2.71053081440314E-3</v>
       </c>
-      <c r="AZ11">
+      <c r="AZ11" s="2">
         <v>1.9945856403650499</v>
       </c>
-      <c r="BA11">
+      <c r="BA11" s="2">
         <v>-0.74727156759746804</v>
       </c>
-      <c r="BB11">
+      <c r="BB11" s="2">
         <v>-0.87493306420466999</v>
       </c>
-      <c r="BC11">
+      <c r="BC11" s="2">
         <v>2.0889587971985799</v>
       </c>
-      <c r="BD11">
+      <c r="BD11" s="2">
         <v>1.5469730901530701</v>
       </c>
-      <c r="BE11">
+      <c r="BE11" s="2">
         <v>-0.117120085232801</v>
       </c>
-      <c r="BF11">
+      <c r="BF11" s="2">
         <v>0.61142718610876601</v>
       </c>
-      <c r="BG11">
+      <c r="BG11" s="2">
         <v>-1.2617758029700401</v>
       </c>
-      <c r="BH11">
+      <c r="BH11" s="2">
         <v>-0.51351821957235499</v>
       </c>
-      <c r="BI11">
+      <c r="BI11" s="2">
         <v>-0.94710965085045995</v>
       </c>
-      <c r="BJ11">
+      <c r="BJ11" s="2">
         <v>-0.31764330429510201</v>
       </c>
-      <c r="BK11">
+      <c r="BK11" s="2">
         <v>-0.84037097944667205</v>
       </c>
-      <c r="BL11">
+      <c r="BL11" s="2">
         <v>-0.69616764028960998</v>
       </c>
-      <c r="BM11">
+      <c r="BM11" s="2">
         <v>0.502278190961579</v>
       </c>
-      <c r="BN11">
+      <c r="BN11" s="2">
         <v>-4.7160692411735101E-2</v>
       </c>
-      <c r="BO11">
+      <c r="BO11" s="2">
         <v>1.08047832041572</v>
       </c>
-      <c r="BP11">
+      <c r="BP11" s="2">
         <v>0.37202606421444701</v>
       </c>
-      <c r="BQ11">
+      <c r="BQ11" s="2">
         <v>-0.15443965056630299</v>
       </c>
-      <c r="BR11">
+      <c r="BR11" s="2">
         <v>-0.95825077830764105</v>
       </c>
-      <c r="BS11">
+      <c r="BS11" s="2">
         <v>-0.35138784876833901</v>
       </c>
-      <c r="BT11">
+      <c r="BT11" s="2">
         <v>0.43464843436110501</v>
       </c>
-      <c r="BU11">
+      <c r="BU11" s="2">
         <v>0.31827525530706602</v>
       </c>
-      <c r="BV11">
+      <c r="BV11" s="2">
         <v>-0.95844782693476804</v>
       </c>
-      <c r="BW11">
+      <c r="BW11" s="2">
         <v>-8.1887827790068299E-2</v>
       </c>
-      <c r="BX11">
+      <c r="BX11" s="2">
         <v>-0.79487050410419402</v>
       </c>
-      <c r="BY11">
+      <c r="BY11" s="2">
         <v>-0.293811825597589</v>
       </c>
-      <c r="BZ11">
+      <c r="BZ11" s="2">
         <v>-0.74446828355484795</v>
       </c>
-      <c r="CA11">
+      <c r="CA11" s="2">
         <v>-0.72307205253550699</v>
       </c>
-      <c r="CB11">
+      <c r="CB11" s="2">
         <v>-0.80807089232289298</v>
       </c>
-      <c r="CC11">
+      <c r="CC11" s="2">
         <v>1.7735057431830099</v>
       </c>
-      <c r="CD11">
+      <c r="CD11" s="2">
         <v>0.94852727544870497</v>
       </c>
-      <c r="CE11">
+      <c r="CE11" s="2">
         <v>1.85539601494127</v>
       </c>
-      <c r="CF11">
+      <c r="CF11" s="2">
         <v>0.15451649249819599</v>
       </c>
-      <c r="CG11">
+      <c r="CG11" s="2">
         <v>2.3688762630475502</v>
       </c>
-      <c r="CH11">
+      <c r="CH11" s="2">
         <v>9.8847995590200799E-3</v>
       </c>
-      <c r="CI11">
+      <c r="CI11" s="2">
         <v>-0.17027361175637901</v>
       </c>
-      <c r="CJ11">
+      <c r="CJ11" s="2">
         <v>-0.80464861294489498</v>
       </c>
-      <c r="CK11">
+      <c r="CK11" s="2">
         <v>-0.95401447201315004</v>
       </c>
-      <c r="CL11">
+      <c r="CL11" s="2">
         <v>-0.93667037882680504</v>
       </c>
-      <c r="CM11">
+      <c r="CM11" s="2">
         <v>0.33775455199443599</v>
       </c>
-      <c r="CN11">
+      <c r="CN11" s="2">
         <v>-0.74268799872520297</v>
       </c>
-      <c r="CO11">
+      <c r="CO11" s="2">
         <v>-0.235175995059553</v>
       </c>
-      <c r="CP11">
+      <c r="CP11" s="2">
         <v>-1.16393492254636</v>
       </c>
-      <c r="CQ11">
+      <c r="CQ11" s="2">
         <v>-0.77473238274173695</v>
       </c>
-      <c r="CR11">
+      <c r="CR11" s="2">
         <v>-0.89606536384190705</v>
       </c>
-      <c r="CS11">
+      <c r="CS11" s="2">
         <v>0.74890522707531504</v>
       </c>
-      <c r="CT11">
+      <c r="CT11" s="2">
         <v>-0.95684502888056699</v>
       </c>
-      <c r="CU11">
+      <c r="CU11" s="2">
         <v>2.0139234999909101</v>
       </c>
-      <c r="CV11">
+      <c r="CV11" s="2">
         <v>-0.50644390647866899</v>
       </c>
-      <c r="CW11">
+      <c r="CW11" s="2">
         <v>-0.888372874711437</v>
       </c>
-      <c r="CX11">
+      <c r="CX11" s="2">
         <v>6.7996476112732102E-2</v>
       </c>
-      <c r="CY11">
+      <c r="CY11" s="2">
         <v>4.2052260218060702E-2</v>
       </c>
-      <c r="CZ11">
+      <c r="CZ11" s="2">
         <v>4.1599650844197297E-2</v>
       </c>
-      <c r="DA11">
+      <c r="DA11" s="2">
         <v>4.6085333031593699E-2</v>
       </c>
-      <c r="DB11">
+      <c r="DB11" s="2">
         <v>2.32204773412432E-2</v>
       </c>
-      <c r="DC11">
+      <c r="DC11" s="2">
         <v>2.0238104859893101E-2</v>
       </c>
-      <c r="DD11">
+      <c r="DD11" s="2">
         <v>1.3085260290801501E-2</v>
       </c>
-      <c r="DE11">
+      <c r="DE11" s="2">
         <v>1.4936109337493E-2</v>
       </c>
-      <c r="DF11">
+      <c r="DF11" s="2">
         <v>1.0013982396728301E-2</v>
       </c>
-      <c r="DG11">
+      <c r="DG11" s="2">
         <v>1.3190330324019801E-2</v>
       </c>
-      <c r="DH11">
+      <c r="DH11" s="2">
         <v>1.4612816927590601E-2</v>
       </c>
-      <c r="DI11">
+      <c r="DI11" s="2">
         <v>1.58979042569528E-2</v>
       </c>
-      <c r="DJ11">
+      <c r="DJ11" s="2">
         <v>4.5988345308622999E-3</v>
       </c>
-      <c r="DK11">
+      <c r="DK11" s="2">
         <v>1.04019332886112E-2</v>
       </c>
-      <c r="DL11">
+      <c r="DL11" s="2">
         <v>6.5305066800294201E-3</v>
       </c>
-      <c r="DM11">
+      <c r="DM11" s="2">
         <v>9.7876777097965703E-3</v>
       </c>
-      <c r="DN11">
+      <c r="DN11" s="2">
         <v>8.7935535493465396E-3</v>
       </c>
-      <c r="DO11">
+      <c r="DO11" s="2">
         <v>1.1420304379803899E-2</v>
       </c>
-      <c r="DP11">
+      <c r="DP11" s="2">
         <v>3.7097804036305701E-3</v>
       </c>
-      <c r="DQ11">
+      <c r="DQ11" s="2">
         <v>2.9904547915976299E-3</v>
       </c>
-      <c r="DR11">
+      <c r="DR11" s="2">
         <v>6.6194120927525902E-3</v>
       </c>
-      <c r="DS11">
+      <c r="DS11" s="2">
         <v>3.8875912290769199E-3</v>
       </c>
-      <c r="DT11">
+      <c r="DT11" s="2">
         <v>5.7222756552732998E-3</v>
       </c>
-      <c r="DU11">
+      <c r="DU11" s="2">
         <v>1.10727650391588E-2</v>
       </c>
-      <c r="DV11">
+      <c r="DV11" s="2">
         <v>8.4864257599392198E-4</v>
       </c>
-      <c r="DW11">
+      <c r="DW11" s="2">
         <v>2.7964793456561601E-3</v>
       </c>
-      <c r="DX11">
+      <c r="DX11" s="2">
         <v>3.71786271387813E-3</v>
       </c>
-      <c r="DY11">
+      <c r="DY11" s="2">
         <v>4.9544561817549898E-3</v>
       </c>
-      <c r="DZ11">
+      <c r="DZ11" s="2">
         <v>6.4981774390391704E-3</v>
       </c>
-      <c r="EA11">
+      <c r="EA11" s="2">
         <v>4.1138959160086303E-3</v>
       </c>
-      <c r="EB11">
+      <c r="EB11" s="2">
         <v>4.2028013287318E-4</v>
       </c>
-      <c r="EC11">
+      <c r="EC11" s="2">
         <v>2.0933183541183399E-3</v>
       </c>
-      <c r="ED11">
+      <c r="ED11" s="2">
         <v>2.1337299053561499E-3</v>
       </c>
-      <c r="EE11">
+      <c r="EE11" s="2">
         <v>1.7134497724829701E-3</v>
       </c>
-      <c r="EF11">
+      <c r="EF11" s="2">
         <v>6.3446135443355096E-3</v>
       </c>
-      <c r="EG11">
+      <c r="EG11" s="2">
         <v>3.2329240990244699E-3</v>
       </c>
-      <c r="EH11">
+      <c r="EH11" s="2">
         <v>1.93975445941468E-3</v>
       </c>
-      <c r="EI11">
+      <c r="EI11" s="2">
         <v>3.6693688523927702E-3</v>
       </c>
-      <c r="EJ11">
+      <c r="EJ11" s="2">
         <v>7.4842192892416396E-3</v>
       </c>
-      <c r="EK11">
+      <c r="EK11" s="2">
         <v>2.2711291795646901E-3</v>
       </c>
-      <c r="EL11">
+      <c r="EL11" s="2">
         <v>2.6105862099622601E-3</v>
       </c>
-      <c r="EM11">
+      <c r="EM11" s="2">
         <v>2.1014006643659E-4</v>
       </c>
-      <c r="EN11">
+      <c r="EN11" s="2">
         <v>5.1807608686867098E-3</v>
       </c>
-      <c r="EO11">
+      <c r="EO11" s="2">
         <v>2.9015493788744598E-3</v>
       </c>
-      <c r="EP11">
+      <c r="EP11" s="2">
         <v>2.7560677944183602E-3</v>
       </c>
-      <c r="EQ11">
+      <c r="EQ11" s="2">
         <v>2.57825696897201E-3</v>
       </c>
-      <c r="ER11">
+      <c r="ER11" s="2">
         <v>3.2975825810049502E-3</v>
       </c>
-      <c r="ES11">
+      <c r="ES11" s="2">
         <v>1.9397544594146801E-4</v>
       </c>
-      <c r="ET11">
+      <c r="ET11" s="2">
         <v>4.4048590849208296E-3</v>
       </c>
-      <c r="EU11">
+      <c r="EU11" s="2">
         <v>4.9706208022501199E-3</v>
       </c>
-      <c r="EV11">
+      <c r="EV11" s="2">
         <v>1.20426422688661E-3</v>
       </c>
-      <c r="EW11">
+      <c r="EW11" s="2">
         <v>6.3850250955733198E-4</v>
       </c>
-      <c r="EX11">
+      <c r="EX11" s="2">
         <v>2.40852845377323E-3</v>
       </c>
-      <c r="EY11">
+      <c r="EY11" s="2">
         <v>1.0668649526780699E-3</v>
       </c>
-      <c r="EZ11">
+      <c r="EZ11" s="2">
         <v>1.7942728749585799E-3</v>
       </c>
-      <c r="FA11">
+      <c r="FA11" s="2">
         <v>2.6025038997146998E-3</v>
       </c>
-      <c r="FB11">
+      <c r="FB11" s="2">
         <v>4.1704720877415603E-3</v>
       </c>
-      <c r="FC11">
+      <c r="FC11" s="2">
         <v>4.5018468078915699E-3</v>
       </c>
-      <c r="FD11">
+      <c r="FD11" s="2">
         <v>3.7986858163537501E-4</v>
       </c>
-      <c r="FE11">
+      <c r="FE11" s="2">
         <v>2.2145530078317602E-3</v>
       </c>
-      <c r="FF11">
+      <c r="FF11" s="2">
         <v>1.8831782876817501E-3</v>
       </c>
-      <c r="FG11">
+      <c r="FG11" s="2">
         <v>1.33358119084759E-3</v>
       </c>
-      <c r="FH11">
+      <c r="FH11" s="2">
         <v>2.65099776120006E-3</v>
       </c>
-      <c r="FI11">
+      <c r="FI11" s="2">
         <v>7.6781947351830995E-4</v>
       </c>
-      <c r="FJ11">
+      <c r="FJ11" s="2">
         <v>1.3416635010951501E-3</v>
       </c>
-      <c r="FK11">
+      <c r="FK11" s="2">
         <v>1.2365934678768599E-3</v>
       </c>
-      <c r="FL11">
+      <c r="FL11" s="2">
         <v>1.3497458113427101E-3</v>
       </c>
-      <c r="FM11">
+      <c r="FM11" s="2">
         <v>1.5598858777793E-3</v>
       </c>
-      <c r="FN11" s="1">
+      <c r="FN11" s="3">
         <v>8.0823102475611603E-6</v>
       </c>
-      <c r="FO11">
+      <c r="FO11" s="2">
         <v>1.4063219830756401E-3</v>
       </c>
-      <c r="FP11">
+      <c r="FP11" s="2">
         <v>1.68112053149272E-3</v>
       </c>
-      <c r="FQ11">
+      <c r="FQ11" s="2">
         <v>2.78031472516104E-3</v>
       </c>
-      <c r="FR11">
+      <c r="FR11" s="2">
         <v>5.2535016609147603E-4</v>
       </c>
-      <c r="FS11">
+      <c r="FS11" s="2">
         <v>1.55180356753174E-3</v>
       </c>
-      <c r="FT11">
+      <c r="FT11" s="2">
         <v>1.4063219830756401E-3</v>
       </c>
-      <c r="FU11">
+      <c r="FU11" s="2">
         <v>8.4864257599392198E-4</v>
       </c>
-      <c r="FV11">
+      <c r="FV11" s="2">
         <v>7.6781947351830995E-4</v>
       </c>
-      <c r="FW11">
+      <c r="FW11" s="2">
         <v>2.9904547915976298E-4</v>
       </c>
-      <c r="FX11">
+      <c r="FX11" s="2">
         <v>2.9904547915976298E-4</v>
       </c>
-      <c r="FY11">
+      <c r="FY11" s="2">
         <v>1.8993429081768699E-3</v>
       </c>
-      <c r="FZ11">
+      <c r="FZ11" s="2">
         <v>5.4151478658659804E-4</v>
       </c>
-      <c r="GA11">
+      <c r="GA11" s="2">
         <v>1.0507003321829501E-3</v>
       </c>
-      <c r="GB11">
+      <c r="GB11" s="2">
         <v>3.8795089188293602E-4</v>
       </c>
-      <c r="GC11">
+      <c r="GC11" s="2">
         <v>7.8398409401343305E-4</v>
       </c>
-      <c r="GD11">
+      <c r="GD11" s="2">
         <v>6.3850250955733198E-4</v>
       </c>
-      <c r="GE11">
+      <c r="GE11" s="2">
         <v>1.1072765039158801E-3</v>
       </c>
-      <c r="GF11" s="1">
+      <c r="GF11" s="3">
         <v>2.4246930742683501E-5</v>
       </c>
-      <c r="GG11">
+      <c r="GG11" s="2">
         <v>3.71786271387814E-4</v>
       </c>
-      <c r="GH11">
+      <c r="GH11" s="2">
         <v>1.6972851519878401E-4</v>
       </c>
-      <c r="GI11">
+      <c r="GI11" s="2">
         <v>1.5437212572841799E-3</v>
       </c>
-      <c r="GJ11">
+      <c r="GJ11" s="2">
         <v>3.0712778940732399E-4</v>
       </c>
-      <c r="GK11">
+      <c r="GK11" s="2">
         <v>1.5356389470366199E-4</v>
       </c>
-      <c r="GL11">
-        <v>0</v>
-      </c>
-      <c r="GM11">
+      <c r="GL11" s="2">
+        <v>0</v>
+      </c>
+      <c r="GM11" s="2">
         <v>3.9603320213049703E-4</v>
       </c>
-      <c r="GN11">
+      <c r="GN11" s="2">
         <v>6.62749440300015E-4</v>
       </c>
-      <c r="GO11">
+      <c r="GO11" s="2">
         <v>1.56796818802687E-3</v>
       </c>
-      <c r="GP11">
+      <c r="GP11" s="2">
         <v>8.4056026574636097E-4</v>
       </c>
-      <c r="GQ11">
+      <c r="GQ11" s="2">
         <v>5.5767940708171995E-4</v>
       </c>
-      <c r="GR11">
+      <c r="GR11" s="2">
         <v>1.05070033218295E-4</v>
       </c>
-      <c r="GS11">
+      <c r="GS11" s="2">
         <v>1.5922151187695501E-3</v>
       </c>
     </row>
@@ -70935,608 +70935,608 @@
         <v>8.4260195483653504E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:201" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:201" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>3.2467403575491001</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>0.79391589660653195</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.79324691667523795</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>2.1940828566825301</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>0.435514070404382</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>-5.1766150236544899E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>1.4282383911493099</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>1.25315094082547</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <v>1.0034833159472201</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <v>0.26669254715512603</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="2">
         <v>1.15850435966753</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="2">
         <v>-0.24607570377160801</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="2">
         <v>0.15820663533585999</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="2">
         <v>1.9978147245109199</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="2">
         <v>0.81710710941875997</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
         <v>-0.62890490062333004</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="2">
         <v>1.16026975614852</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="2">
         <v>2.0242058839005401</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="2">
         <v>-0.119999154856871</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="2">
         <v>1.30975945407495</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="2">
         <v>0.35480817338551102</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="2">
         <v>0.25285243723357798</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="2">
         <v>0.143920446565696</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="2">
         <v>0.95163666604457098</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="2">
         <v>-0.64728949016159398</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="2">
         <v>1.5675945919712999</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="2">
         <v>0.92333784632661298</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" s="2">
         <v>-0.180232963167236</v>
       </c>
-      <c r="AD13">
+      <c r="AD13" s="2">
         <v>0.226499483744865</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="2">
         <v>-0.63503675091870404</v>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="2">
         <v>0.63925134691398899</v>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="2">
         <v>1.71496476213717</v>
       </c>
-      <c r="AH13">
+      <c r="AH13" s="2">
         <v>-0.88203245303998601</v>
       </c>
-      <c r="AI13">
+      <c r="AI13" s="2">
         <v>-0.123354204821195</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="2">
         <v>-6.8036806183043502E-2</v>
       </c>
-      <c r="AK13">
+      <c r="AK13" s="2">
         <v>1.90153640085474</v>
       </c>
-      <c r="AL13">
+      <c r="AL13" s="2">
         <v>8.06749219758012E-2</v>
       </c>
-      <c r="AM13">
+      <c r="AM13" s="2">
         <v>-0.129899662208284</v>
       </c>
-      <c r="AN13">
+      <c r="AN13" s="2">
         <v>-6.0024359327479099E-2</v>
       </c>
-      <c r="AO13">
+      <c r="AO13" s="2">
         <v>2.2188514722983399</v>
       </c>
-      <c r="AP13">
+      <c r="AP13" s="2">
         <v>-0.41348450147389998</v>
       </c>
-      <c r="AQ13">
+      <c r="AQ13" s="2">
         <v>0.86770233470886604</v>
       </c>
-      <c r="AR13">
+      <c r="AR13" s="2">
         <v>-4.5415832199229803E-2</v>
       </c>
-      <c r="AS13">
+      <c r="AS13" s="2">
         <v>-0.93559054367426997</v>
       </c>
-      <c r="AT13">
+      <c r="AT13" s="2">
         <v>0.164606145410997</v>
       </c>
-      <c r="AU13">
+      <c r="AU13" s="2">
         <v>1.1802714073885101</v>
       </c>
-      <c r="AV13">
+      <c r="AV13" s="2">
         <v>1.3616412879077799</v>
       </c>
-      <c r="AW13">
+      <c r="AW13" s="2">
         <v>-1.05017436459792</v>
       </c>
-      <c r="AX13">
+      <c r="AX13" s="2">
         <v>0.16270109282244699</v>
       </c>
-      <c r="AY13">
+      <c r="AY13" s="2">
         <v>0.247954044257439</v>
       </c>
-      <c r="AZ13">
+      <c r="AZ13" s="2">
         <v>1.7530625007137499</v>
       </c>
-      <c r="BA13">
+      <c r="BA13" s="2">
         <v>-0.980893211811937</v>
       </c>
-      <c r="BB13">
+      <c r="BB13" s="2">
         <v>-1.10853843193524</v>
       </c>
-      <c r="BC13">
+      <c r="BC13" s="2">
         <v>1.86263568339686</v>
       </c>
-      <c r="BD13">
+      <c r="BD13" s="2">
         <v>1.76541561056254</v>
       </c>
-      <c r="BE13">
+      <c r="BE13" s="2">
         <v>-0.331469940546051</v>
       </c>
-      <c r="BF13">
+      <c r="BF13" s="2">
         <v>0.39791337688565798</v>
       </c>
-      <c r="BG13">
+      <c r="BG13" s="2">
         <v>-1.05710454550039</v>
       </c>
-      <c r="BH13">
+      <c r="BH13" s="2">
         <v>-0.31394907772493402</v>
       </c>
-      <c r="BI13">
+      <c r="BI13" s="2">
         <v>-1.1465084584754699</v>
       </c>
-      <c r="BJ13">
+      <c r="BJ13" s="2">
         <v>-0.119426492024383</v>
       </c>
-      <c r="BK13">
+      <c r="BK13" s="2">
         <v>-0.64343711772953005</v>
       </c>
-      <c r="BL13">
+      <c r="BL13" s="2">
         <v>-0.89230445739064801</v>
       </c>
-      <c r="BM13">
+      <c r="BM13" s="2">
         <v>0.309658925744069</v>
       </c>
-      <c r="BN13">
+      <c r="BN13" s="2">
         <v>-0.220646810956939</v>
       </c>
-      <c r="BO13">
+      <c r="BO13" s="2">
         <v>1.2514410376137901</v>
       </c>
-      <c r="BP13">
+      <c r="BP13" s="2">
         <v>0.52789004005460605</v>
       </c>
-      <c r="BQ13">
+      <c r="BQ13" s="2">
         <v>-0.30289930720191099</v>
       </c>
-      <c r="BR13">
+      <c r="BR13" s="2">
         <v>-1.1060015944175301</v>
       </c>
-      <c r="BS13">
+      <c r="BS13" s="2">
         <v>-0.494632330764254</v>
       </c>
-      <c r="BT13">
+      <c r="BT13" s="2">
         <v>0.30153432184304602</v>
       </c>
-      <c r="BU13">
+      <c r="BU13" s="2">
         <v>0.44891626659939998</v>
       </c>
-      <c r="BV13">
+      <c r="BV13" s="2">
         <v>-1.0890633717838001</v>
       </c>
-      <c r="BW13">
+      <c r="BW13" s="2">
         <v>-0.20324671400109701</v>
       </c>
-      <c r="BX13">
+      <c r="BX13" s="2">
         <v>-0.91376170352052399</v>
       </c>
-      <c r="BY13">
+      <c r="BY13" s="2">
         <v>-0.38849397182072698</v>
       </c>
-      <c r="BZ13">
+      <c r="BZ13" s="2">
         <v>-0.83640779691770295</v>
       </c>
-      <c r="CA13">
+      <c r="CA13" s="2">
         <v>-0.81308550409309399</v>
       </c>
-      <c r="CB13">
+      <c r="CB13" s="2">
         <v>-0.72470170691236602</v>
       </c>
-      <c r="CC13">
+      <c r="CC13" s="2">
         <v>1.85420474205788</v>
       </c>
-      <c r="CD13">
+      <c r="CD13" s="2">
         <v>1.01757323826554</v>
       </c>
-      <c r="CE13">
+      <c r="CE13" s="2">
         <v>1.7878606453653301</v>
       </c>
-      <c r="CF13">
+      <c r="CF13" s="2">
         <v>0.22189354814451101</v>
       </c>
-      <c r="CG13">
+      <c r="CG13" s="2">
         <v>2.3018883254465301</v>
       </c>
-      <c r="CH13">
+      <c r="CH13" s="2">
         <v>-5.6731765046109599E-2</v>
       </c>
-      <c r="CI13">
+      <c r="CI13" s="2">
         <v>-0.22640458342463099</v>
       </c>
-      <c r="CJ13">
+      <c r="CJ13" s="2">
         <v>-0.85647357020903403</v>
       </c>
-      <c r="CK13">
+      <c r="CK13" s="2">
         <v>-1.00480040581997</v>
       </c>
-      <c r="CL13">
+      <c r="CL13" s="2">
         <v>-0.984783460858074</v>
       </c>
-      <c r="CM13">
+      <c r="CM13" s="2">
         <v>0.29011255686813298</v>
       </c>
-      <c r="CN13">
+      <c r="CN13" s="2">
         <v>-0.69867472557439603</v>
       </c>
-      <c r="CO13">
+      <c r="CO13" s="2">
         <v>-0.27756380991744301</v>
       </c>
-      <c r="CP13">
+      <c r="CP13" s="2">
         <v>-1.1221549330928</v>
       </c>
-      <c r="CQ13">
+      <c r="CQ13" s="2">
         <v>-0.74334995930487502</v>
       </c>
-      <c r="CR13">
+      <c r="CR13" s="2">
         <v>-0.92039574038984995</v>
       </c>
-      <c r="CS13">
+      <c r="CS13" s="2">
         <v>0.764139964450256</v>
       </c>
-      <c r="CT13">
+      <c r="CT13" s="2">
         <v>-0.94203684858440495</v>
       </c>
-      <c r="CU13">
+      <c r="CU13" s="2">
         <v>1.99986782418894</v>
       </c>
-      <c r="CV13">
+      <c r="CV13" s="2">
         <v>-0.49684822056918398</v>
       </c>
-      <c r="CW13">
+      <c r="CW13" s="2">
         <v>-0.89385541385265199</v>
       </c>
-      <c r="CX13">
+      <c r="CX13" s="2">
         <v>6.8238503904142406E-2</v>
       </c>
-      <c r="CY13">
+      <c r="CY13" s="2">
         <v>4.35105722342689E-2</v>
       </c>
-      <c r="CZ13">
+      <c r="CZ13" s="2">
         <v>4.2044610043877099E-2</v>
       </c>
-      <c r="DA13">
+      <c r="DA13" s="2">
         <v>4.2044610043877099E-2</v>
       </c>
-      <c r="DB13">
+      <c r="DB13" s="2">
         <v>2.3638640320068401E-2</v>
       </c>
-      <c r="DC13">
+      <c r="DC13" s="2">
         <v>1.7561005405735599E-2</v>
       </c>
-      <c r="DD13">
+      <c r="DD13" s="2">
         <v>1.1401928147492101E-2</v>
       </c>
-      <c r="DE13">
+      <c r="DE13" s="2">
         <v>1.25217603762636E-2</v>
       </c>
-      <c r="DF13">
+      <c r="DF13" s="2">
         <v>9.4778527726027996E-3</v>
       </c>
-      <c r="DG13">
+      <c r="DG13" s="2">
         <v>1.2134909242687999E-2</v>
       </c>
-      <c r="DH13">
+      <c r="DH13" s="2">
         <v>1.5504586221991501E-2</v>
       </c>
-      <c r="DI13">
+      <c r="DI13" s="2">
         <v>1.4018263445622001E-2</v>
       </c>
-      <c r="DJ13">
+      <c r="DJ13" s="2">
         <v>4.9985238575166197E-3</v>
       </c>
-      <c r="DK13">
+      <c r="DK13" s="2">
         <v>8.7550519703957098E-3</v>
       </c>
-      <c r="DL13">
+      <c r="DL13" s="2">
         <v>8.6125278685520602E-3</v>
       </c>
-      <c r="DM13">
+      <c r="DM13" s="2">
         <v>8.0424314611774496E-3</v>
       </c>
-      <c r="DN13">
+      <c r="DN13" s="2">
         <v>1.14935507843916E-2</v>
       </c>
-      <c r="DO13">
+      <c r="DO13" s="2">
         <v>8.3071190788870895E-3</v>
       </c>
-      <c r="DP13">
+      <c r="DP13" s="2">
         <v>4.1841004184100397E-3</v>
       </c>
-      <c r="DQ13">
+      <c r="DQ13" s="2">
         <v>2.3618279734090699E-3</v>
       </c>
-      <c r="DR13">
+      <c r="DR13" s="2">
         <v>7.1058445062048897E-3</v>
       </c>
-      <c r="DS13">
+      <c r="DS13" s="2">
         <v>3.7056266479349302E-3</v>
       </c>
-      <c r="DT13">
+      <c r="DT13" s="2">
         <v>5.1308676663714397E-3</v>
       </c>
-      <c r="DU13">
+      <c r="DU13" s="2">
         <v>1.08725529120728E-2</v>
       </c>
-      <c r="DV13">
+      <c r="DV13" s="2">
         <v>6.8207963025175903E-4</v>
       </c>
-      <c r="DW13">
+      <c r="DW13" s="2">
         <v>4.2655427623207003E-3</v>
       </c>
-      <c r="DX13">
+      <c r="DX13" s="2">
         <v>2.8403017438841899E-3</v>
       </c>
-      <c r="DY13">
+      <c r="DY13" s="2">
         <v>6.2914210670983097E-3</v>
       </c>
-      <c r="DZ13">
+      <c r="DZ13" s="2">
         <v>4.5302303800303402E-3</v>
       </c>
-      <c r="EA13">
+      <c r="EA13" s="2">
         <v>6.1387166722658296E-3</v>
       </c>
-      <c r="EB13">
+      <c r="EB13" s="2">
         <v>2.6468761770963799E-4</v>
       </c>
-      <c r="EC13">
+      <c r="EC13" s="2">
         <v>1.8222724450009701E-3</v>
       </c>
-      <c r="ED13">
+      <c r="ED13" s="2">
         <v>1.8629936169562999E-3</v>
       </c>
-      <c r="EE13">
+      <c r="EE13" s="2">
         <v>2.9624652597501802E-3</v>
       </c>
-      <c r="EF13">
+      <c r="EF13" s="2">
         <v>5.3446538191369098E-3</v>
       </c>
-      <c r="EG13">
+      <c r="EG13" s="2">
         <v>2.3516476804202398E-3</v>
       </c>
-      <c r="EH13">
+      <c r="EH13" s="2">
         <v>1.8528133239674601E-3</v>
       </c>
-      <c r="EI13">
+      <c r="EI13" s="2">
         <v>3.8685113357562399E-3</v>
       </c>
-      <c r="EJ13">
+      <c r="EJ13" s="2">
         <v>7.2992700729926996E-3</v>
       </c>
-      <c r="EK13">
+      <c r="EK13" s="2">
         <v>2.5756141261745499E-3</v>
       </c>
-      <c r="EL13">
+      <c r="EL13" s="2">
         <v>2.7384988139958701E-3</v>
       </c>
-      <c r="EM13">
+      <c r="EM13" s="2">
         <v>2.8504820368730198E-4</v>
       </c>
-      <c r="EN13">
+      <c r="EN13" s="2">
         <v>5.73150495271254E-3</v>
       </c>
-      <c r="EO13">
+      <c r="EO13" s="2">
         <v>2.3414673874314102E-3</v>
       </c>
-      <c r="EP13">
+      <c r="EP13" s="2">
         <v>1.9647965468446199E-3</v>
       </c>
-      <c r="EQ13">
+      <c r="EQ13" s="2">
         <v>2.1480418206435998E-3</v>
       </c>
-      <c r="ER13">
+      <c r="ER13" s="2">
         <v>2.1378615276547702E-3</v>
       </c>
-      <c r="ES13">
+      <c r="ES13" s="2">
         <v>1.4252410184365099E-4</v>
       </c>
-      <c r="ET13">
+      <c r="ET13" s="2">
         <v>4.3877062781866897E-3</v>
       </c>
-      <c r="EU13">
+      <c r="EU13" s="2">
         <v>4.63203330991866E-3</v>
       </c>
-      <c r="EV13">
+      <c r="EV13" s="2">
         <v>1.6899286361461499E-3</v>
       </c>
-      <c r="EW13">
+      <c r="EW13" s="2">
         <v>4.7847377047511398E-4</v>
       </c>
-      <c r="EX13">
+      <c r="EX13" s="2">
         <v>1.56776512028016E-3</v>
       </c>
-      <c r="EY13">
+      <c r="EY13" s="2">
         <v>9.5694754095022796E-4</v>
       </c>
-      <c r="EZ13">
+      <c r="EZ13" s="2">
         <v>2.1276812346659301E-3</v>
       </c>
-      <c r="FA13">
+      <c r="FA13" s="2">
         <v>3.1660711195268202E-3</v>
       </c>
-      <c r="FB13">
+      <c r="FB13" s="2">
         <v>2.8912032088283502E-3</v>
       </c>
-      <c r="FC13">
+      <c r="FC13" s="2">
         <v>4.1535595394435404E-3</v>
       </c>
-      <c r="FD13">
+      <c r="FD13" s="2">
         <v>3.0337273106719998E-3</v>
       </c>
-      <c r="FE13">
+      <c r="FE13" s="2">
         <v>2.1276812346659301E-3</v>
       </c>
-      <c r="FF13">
+      <c r="FF13" s="2">
         <v>1.3132577955593599E-3</v>
       </c>
-      <c r="FG13">
+      <c r="FG13" s="2">
         <v>1.0994716427938801E-3</v>
       </c>
-      <c r="FH13">
+      <c r="FH13" s="2">
         <v>1.8019118590233E-3</v>
       </c>
-      <c r="FI13">
+      <c r="FI13" s="2">
         <v>5.5991611438577205E-4</v>
       </c>
-      <c r="FJ13">
+      <c r="FJ13" s="2">
         <v>1.53722424131367E-3</v>
       </c>
-      <c r="FK13">
+      <c r="FK13" s="2">
         <v>1.1809139867045399E-3</v>
       </c>
-      <c r="FL13">
+      <c r="FL13" s="2">
         <v>1.15037310773804E-3</v>
       </c>
-      <c r="FM13">
+      <c r="FM13" s="2">
         <v>1.62884687821315E-3</v>
       </c>
-      <c r="FN13">
-        <v>0</v>
-      </c>
-      <c r="FO13">
+      <c r="FN13" s="2">
+        <v>0</v>
+      </c>
+      <c r="FO13" s="2">
         <v>9.5694754095022796E-4</v>
       </c>
-      <c r="FP13">
+      <c r="FP13" s="2">
         <v>2.4941717822638898E-3</v>
       </c>
-      <c r="FQ13">
+      <c r="FQ13" s="2">
         <v>2.1276812346659301E-3</v>
       </c>
-      <c r="FR13">
+      <c r="FR13" s="2">
         <v>2.1378615276547699E-4</v>
       </c>
-      <c r="FS13">
+      <c r="FS13" s="2">
         <v>1.4557818974030099E-3</v>
       </c>
-      <c r="FT13">
+      <c r="FT13" s="2">
         <v>1.19109427969337E-3</v>
       </c>
-      <c r="FU13">
+      <c r="FU13" s="2">
         <v>8.55144611061906E-4</v>
       </c>
-      <c r="FV13">
+      <c r="FV13" s="2">
         <v>1.11983222877154E-3</v>
       </c>
-      <c r="FW13">
+      <c r="FW13" s="2">
         <v>3.8685113357562399E-4</v>
       </c>
-      <c r="FX13">
+      <c r="FX13" s="2">
         <v>2.4432703173197303E-4</v>
       </c>
-      <c r="FY13">
+      <c r="FY13" s="2">
         <v>2.78940027894003E-3</v>
       </c>
-      <c r="FZ13">
+      <c r="FZ13" s="2">
         <v>4.1739201254212098E-4</v>
       </c>
-      <c r="GA13">
+      <c r="GA13" s="2">
         <v>7.3298109519592E-4</v>
       </c>
-      <c r="GB13">
+      <c r="GB13" s="2">
         <v>2.7486791069847001E-4</v>
       </c>
-      <c r="GC13">
+      <c r="GC13" s="2">
         <v>1.2419957446375301E-3</v>
       </c>
-      <c r="GD13">
+      <c r="GD13" s="2">
         <v>5.8027670036343599E-4</v>
       </c>
-      <c r="GE13">
+      <c r="GE13" s="2">
         <v>1.0689307638273801E-3</v>
       </c>
-      <c r="GF13" s="1">
+      <c r="GF13" s="3">
         <v>4.0721171955328901E-5</v>
       </c>
-      <c r="GG13">
+      <c r="GG13" s="2">
         <v>1.8324527379898E-4</v>
       </c>
-      <c r="GH13">
+      <c r="GH13" s="2">
         <v>2.31092650846491E-3</v>
       </c>
-      <c r="GI13">
+      <c r="GI13" s="2">
         <v>1.6797483431573201E-3</v>
       </c>
-      <c r="GJ13">
+      <c r="GJ13" s="2">
         <v>3.3594966863146301E-4</v>
       </c>
-      <c r="GK13" s="1">
+      <c r="GK13" s="3">
         <v>5.0901464944161099E-5</v>
       </c>
-      <c r="GL13">
+      <c r="GL13" s="2">
         <v>7.0345824552830597E-3</v>
       </c>
-      <c r="GM13">
+      <c r="GM13" s="2">
         <v>5.2937523541927501E-4</v>
       </c>
-      <c r="GN13">
+      <c r="GN13" s="2">
         <v>3.1558908265379902E-4</v>
       </c>
-      <c r="GO13">
+      <c r="GO13" s="2">
         <v>1.16055340072687E-3</v>
       </c>
-      <c r="GP13">
+      <c r="GP13" s="2">
         <v>6.7189933726292603E-4</v>
       </c>
-      <c r="GQ13">
+      <c r="GQ13" s="2">
         <v>7.94062853128913E-4</v>
       </c>
-      <c r="GR13">
+      <c r="GR13" s="2">
         <v>1.5270439483248301E-4</v>
       </c>
-      <c r="GS13">
+      <c r="GS13" s="2">
         <v>2.0258783047776099E-3</v>
       </c>
     </row>
@@ -72145,1213 +72145,1213 @@
         <v>1.4537701104865299E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:201" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:201" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4">
         <v>-0.36458910873510703</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>-0.72647902695936395</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>-0.57204338482477302</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="4">
         <v>-0.37609145327678201</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="4">
         <v>-0.45145726670180503</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="4">
         <v>-0.59400876486989396</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="4">
         <v>-0.29076589573121198</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="4">
         <v>-0.69876641281195795</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="4">
         <v>-0.94101754811808802</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="4">
         <v>0.388493768589871</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="4">
         <v>-0.74805175401017998</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="4">
         <v>0.88145437218674105</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="4">
         <v>8.8781536596680394E-2</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="4">
         <v>-1.19299606711103</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="4">
         <v>-0.87526869649117101</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="4">
         <v>-0.48032019066757098</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="4">
         <v>-0.96429037583116395</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="4">
         <v>-1.0380442369029399</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="4">
         <v>0.31907438151401002</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="4">
         <v>-0.91784227852969402</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15" s="4">
         <v>-1.0114782553255699</v>
       </c>
-      <c r="W15" s="2">
+      <c r="W15" s="4">
         <v>-0.93842179919258595</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15" s="4">
         <v>-0.33587940909116598</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Y15" s="4">
         <v>-0.52729061107361797</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="Z15" s="4">
         <v>1.5503992933998101</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AA15" s="4">
         <v>-0.79289819127529204</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AB15" s="4">
         <v>0.14977645854232699</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AC15" s="4">
         <v>-0.83482279561081796</v>
       </c>
-      <c r="AD15" s="2">
+      <c r="AD15" s="4">
         <v>-0.64844149156238096</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AE15" s="4">
         <v>0.47279026964680798</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="AF15" s="4">
         <v>1.3148672877504999E-2</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="AG15" s="4">
         <v>-0.719824368618868</v>
       </c>
-      <c r="AH15" s="2">
+      <c r="AH15" s="4">
         <v>-0.14462978520970299</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="AI15" s="4">
         <v>-0.17438142562994699</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="AJ15" s="4">
         <v>-0.528653300061942</v>
       </c>
-      <c r="AK15" s="2">
+      <c r="AK15" s="4">
         <v>-0.79530006220175997</v>
       </c>
-      <c r="AL15" s="2">
+      <c r="AL15" s="4">
         <v>-0.59470587256478802</v>
       </c>
-      <c r="AM15" s="2">
+      <c r="AM15" s="4">
         <v>-0.63361990668227897</v>
       </c>
-      <c r="AN15" s="2">
+      <c r="AN15" s="4">
         <v>-0.57620372770921202</v>
       </c>
-      <c r="AO15" s="2">
+      <c r="AO15" s="4">
         <v>-0.78883357038809998</v>
       </c>
-      <c r="AP15" s="2">
+      <c r="AP15" s="4">
         <v>0.81007859131724502</v>
       </c>
-      <c r="AQ15" s="2">
+      <c r="AQ15" s="4">
         <v>-0.94033138671957495</v>
       </c>
-      <c r="AR15" s="2">
+      <c r="AR15" s="4">
         <v>0.29810275467506803</v>
       </c>
-      <c r="AS15" s="2">
+      <c r="AS15" s="4">
         <v>0.109397001694684</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AT15" s="4">
         <v>-0.262610803254826</v>
       </c>
-      <c r="AU15" s="2">
+      <c r="AU15" s="4">
         <v>0.74385979686067205</v>
       </c>
-      <c r="AV15" s="2">
+      <c r="AV15" s="4">
         <v>-1.2676571828718599</v>
       </c>
-      <c r="AW15" s="2">
+      <c r="AW15" s="4">
         <v>0.49315658400229301</v>
       </c>
-      <c r="AX15" s="2">
+      <c r="AX15" s="4">
         <v>-0.116008190645357</v>
       </c>
-      <c r="AY15" s="2">
+      <c r="AY15" s="4">
         <v>-0.41452648385825902</v>
       </c>
-      <c r="AZ15" s="2">
+      <c r="AZ15" s="4">
         <v>-0.79205918707591505</v>
       </c>
-      <c r="BA15" s="2">
+      <c r="BA15" s="4">
         <v>2.3592807987346101</v>
       </c>
-      <c r="BB15" s="2">
+      <c r="BB15" s="4">
         <v>1.1522171890317301</v>
       </c>
-      <c r="BC15" s="2">
+      <c r="BC15" s="4">
         <v>-0.239394635091671</v>
       </c>
-      <c r="BD15" s="2">
+      <c r="BD15" s="4">
         <v>-0.71181694621114699</v>
       </c>
-      <c r="BE15" s="2">
+      <c r="BE15" s="4">
         <v>-7.8490747252030299E-2</v>
       </c>
-      <c r="BF15" s="2">
+      <c r="BF15" s="4">
         <v>-0.80831819858374998</v>
       </c>
-      <c r="BG15" s="2">
+      <c r="BG15" s="4">
         <v>1.5242136297482101</v>
       </c>
-      <c r="BH15" s="2">
+      <c r="BH15" s="4">
         <v>-0.43170962107356697</v>
       </c>
-      <c r="BI15" s="2">
+      <c r="BI15" s="4">
         <v>1.46829142574352</v>
       </c>
-      <c r="BJ15" s="2">
+      <c r="BJ15" s="4">
         <v>-0.50466463384949201</v>
       </c>
-      <c r="BK15" s="2">
+      <c r="BK15" s="4">
         <v>0.386948516306861</v>
       </c>
-      <c r="BL15" s="2">
+      <c r="BL15" s="4">
         <v>2.5784427698225101</v>
       </c>
-      <c r="BM15" s="2">
+      <c r="BM15" s="4">
         <v>-0.74381609838650398</v>
       </c>
-      <c r="BN15" s="2">
+      <c r="BN15" s="4">
         <v>0.29903751748749302</v>
       </c>
-      <c r="BO15" s="2">
+      <c r="BO15" s="4">
         <v>3.7158704136171297E-2</v>
       </c>
-      <c r="BP15" s="2">
+      <c r="BP15" s="4">
         <v>-0.380265249314723</v>
       </c>
-      <c r="BQ15" s="2">
+      <c r="BQ15" s="4">
         <v>0.89253384198342001</v>
       </c>
-      <c r="BR15" s="2">
+      <c r="BR15" s="4">
         <v>2.0327831674877501</v>
       </c>
-      <c r="BS15" s="2">
+      <c r="BS15" s="4">
         <v>-0.77016100229382001</v>
       </c>
-      <c r="BT15" s="2">
+      <c r="BT15" s="4">
         <v>-1.1495932302315801</v>
       </c>
-      <c r="BU15" s="2">
+      <c r="BU15" s="4">
         <v>-1.0739247496076501</v>
       </c>
-      <c r="BV15" s="2">
+      <c r="BV15" s="4">
         <v>0.31098510417177799</v>
       </c>
-      <c r="BW15" s="2">
+      <c r="BW15" s="4">
         <v>-0.52617876550924803</v>
       </c>
-      <c r="BX15" s="2">
+      <c r="BX15" s="4">
         <v>-0.13899496756888699</v>
       </c>
-      <c r="BY15" s="2">
+      <c r="BY15" s="4">
         <v>0.95308165905064801</v>
       </c>
-      <c r="BZ15" s="2">
+      <c r="BZ15" s="4">
         <v>2.68103370069948</v>
       </c>
-      <c r="CA15" s="2">
+      <c r="CA15" s="4">
         <v>2.3711084213365501</v>
       </c>
-      <c r="CB15" s="2">
+      <c r="CB15" s="4">
         <v>1.8029462594501899</v>
       </c>
-      <c r="CC15" s="2">
+      <c r="CC15" s="4">
         <v>-1.02856289972648</v>
       </c>
-      <c r="CD15" s="2">
+      <c r="CD15" s="4">
         <v>-0.93117239051933298</v>
       </c>
-      <c r="CE15" s="2">
+      <c r="CE15" s="4">
         <v>-0.72816000258135605</v>
       </c>
-      <c r="CF15" s="2">
+      <c r="CF15" s="4">
         <v>-0.26088269303794798</v>
       </c>
-      <c r="CG15" s="2">
+      <c r="CG15" s="4">
         <v>-0.40283737365119299</v>
       </c>
-      <c r="CH15" s="2">
+      <c r="CH15" s="4">
         <v>-0.68640811990445005</v>
       </c>
-      <c r="CI15" s="2">
+      <c r="CI15" s="4">
         <v>0.30739372707863699</v>
       </c>
-      <c r="CJ15" s="2">
+      <c r="CJ15" s="4">
         <v>2.2224977148792999</v>
       </c>
-      <c r="CK15" s="2">
+      <c r="CK15" s="4">
         <v>2.1997572422849401</v>
       </c>
-      <c r="CL15" s="2">
+      <c r="CL15" s="4">
         <v>0.94550357658986295</v>
       </c>
-      <c r="CM15" s="2">
+      <c r="CM15" s="4">
         <v>-0.81556949015821101</v>
       </c>
-      <c r="CN15" s="2">
+      <c r="CN15" s="4">
         <v>1.1185452282477999</v>
       </c>
-      <c r="CO15" s="2">
+      <c r="CO15" s="4">
         <v>-0.76394177979978195</v>
       </c>
-      <c r="CP15" s="2">
+      <c r="CP15" s="4">
         <v>1.1453008244426199</v>
       </c>
-      <c r="CQ15" s="2">
+      <c r="CQ15" s="4">
         <v>0.38885000064869402</v>
       </c>
-      <c r="CR15" s="2">
+      <c r="CR15" s="4">
         <v>0.57710771936771599</v>
       </c>
-      <c r="CS15" s="2">
+      <c r="CS15" s="4">
         <v>-1.1930265711558601</v>
       </c>
-      <c r="CT15" s="2">
+      <c r="CT15" s="4">
         <v>2.2967797979919902</v>
       </c>
-      <c r="CU15" s="2">
+      <c r="CU15" s="4">
         <v>-0.74245128729346399</v>
       </c>
-      <c r="CV15" s="2">
+      <c r="CV15" s="4">
         <v>0.27149161555752299</v>
       </c>
-      <c r="CW15" s="2">
+      <c r="CW15" s="4">
         <v>1.7293008482804799</v>
       </c>
-      <c r="CX15" s="2">
+      <c r="CX15" s="4">
         <v>3.71458317840411E-2</v>
       </c>
-      <c r="CY15" s="2">
+      <c r="CY15" s="4">
         <v>2.6511489551572801E-2</v>
       </c>
-      <c r="CZ15" s="2">
+      <c r="CZ15" s="4">
         <v>2.9486130735479999E-2</v>
       </c>
-      <c r="DA15" s="2">
+      <c r="DA15" s="4">
         <v>1.5579683200713901E-2</v>
       </c>
-      <c r="DB15" s="2">
+      <c r="DB15" s="4">
         <v>8.7008254629285294E-3</v>
       </c>
-      <c r="DC15" s="2">
+      <c r="DC15" s="4">
         <v>1.4055179593961501E-2</v>
       </c>
-      <c r="DD15" s="2">
+      <c r="DD15" s="4">
         <v>1.7587565999851298E-2</v>
       </c>
-      <c r="DE15" s="2">
+      <c r="DE15" s="4">
         <v>8.5892764185320093E-3</v>
       </c>
-      <c r="DF15" s="2">
+      <c r="DF15" s="4">
         <v>1.3794898490369601E-2</v>
       </c>
-      <c r="DG15" s="2">
+      <c r="DG15" s="4">
         <v>6.1723804566074202E-3</v>
       </c>
-      <c r="DH15" s="2">
+      <c r="DH15" s="4">
         <v>5.3915371458317799E-3</v>
       </c>
-      <c r="DI15" s="2">
+      <c r="DI15" s="4">
         <v>4.4247787610619503E-3</v>
       </c>
-      <c r="DJ15" s="2">
+      <c r="DJ15" s="4">
         <v>1.0039413995686799E-2</v>
       </c>
-      <c r="DK15" s="2">
+      <c r="DK15" s="4">
         <v>6.5070275897969798E-3</v>
       </c>
-      <c r="DL15" s="2">
+      <c r="DL15" s="4">
         <v>2.9746411839071899E-3</v>
       </c>
-      <c r="DM15" s="2">
+      <c r="DM15" s="4">
         <v>4.1273146426712296E-3</v>
       </c>
-      <c r="DN15" s="2">
+      <c r="DN15" s="4">
         <v>1.5988696363501199E-3</v>
       </c>
-      <c r="DO15" s="2">
+      <c r="DO15" s="4">
         <v>1.89633375474083E-3</v>
       </c>
-      <c r="DP15" s="2">
+      <c r="DP15" s="4">
         <v>3.9042165538781901E-3</v>
       </c>
-      <c r="DQ15" s="2">
+      <c r="DQ15" s="4">
         <v>1.1526734587640401E-3</v>
       </c>
-      <c r="DR15" s="2">
+      <c r="DR15" s="4">
         <v>2.0450658139361901E-3</v>
       </c>
-      <c r="DS15" s="2">
+      <c r="DS15" s="4">
         <v>6.2839295010039403E-3</v>
       </c>
-      <c r="DT15" s="2">
+      <c r="DT15" s="4">
         <v>1.89633375474083E-3</v>
       </c>
-      <c r="DU15" s="2">
+      <c r="DU15" s="4">
         <v>2.7887261099129898E-3</v>
       </c>
-      <c r="DV15" s="2">
+      <c r="DV15" s="4">
         <v>1.11920874544508E-2</v>
       </c>
-      <c r="DW15" s="2">
+      <c r="DW15" s="4">
         <v>3.1977392727002298E-3</v>
       </c>
-      <c r="DX15" s="2">
+      <c r="DX15" s="4">
         <v>4.7222428794526702E-3</v>
       </c>
-      <c r="DY15" s="2">
+      <c r="DY15" s="4">
         <v>2.1937978731315501E-3</v>
       </c>
-      <c r="DZ15" s="2">
+      <c r="DZ15" s="4">
         <v>1.00394139956868E-3</v>
       </c>
-      <c r="EA15" s="2">
+      <c r="EA15" s="4">
         <v>1.85915073994199E-3</v>
       </c>
-      <c r="EB15" s="2">
+      <c r="EB15" s="4">
         <v>6.5070275897969798E-3</v>
       </c>
-      <c r="EC15" s="2">
+      <c r="EC15" s="4">
         <v>6.6185766341934999E-3</v>
       </c>
-      <c r="ED15" s="2">
+      <c r="ED15" s="4">
         <v>3.5323864058897899E-3</v>
       </c>
-      <c r="EE15" s="2">
+      <c r="EE15" s="4">
         <v>2.8630921395106702E-3</v>
       </c>
-      <c r="EF15" s="2">
+      <c r="EF15" s="4">
         <v>1.2270394883617201E-3</v>
       </c>
-      <c r="EG15" s="2">
+      <c r="EG15" s="4">
         <v>2.8630921395106702E-3</v>
       </c>
-      <c r="EH15" s="2">
+      <c r="EH15" s="4">
         <v>8.5520934037331699E-4</v>
       </c>
-      <c r="EI15" s="2">
+      <c r="EI15" s="4">
         <v>2.4540789767234302E-3</v>
       </c>
-      <c r="EJ15" s="2">
+      <c r="EJ15" s="4">
         <v>4.0901316278723899E-4</v>
       </c>
-      <c r="EK15" s="2">
+      <c r="EK15" s="4">
         <v>2.2309808879303898E-3</v>
       </c>
-      <c r="EL15" s="2">
+      <c r="EL15" s="4">
         <v>1.82196772514315E-3</v>
       </c>
-      <c r="EM15" s="2">
+      <c r="EM15" s="4">
         <v>4.3504127314642699E-3</v>
       </c>
-      <c r="EN15" s="2">
+      <c r="EN15" s="4">
         <v>1.0411244143675199E-3</v>
       </c>
-      <c r="EO15" s="2">
+      <c r="EO15" s="4">
         <v>1.41295456235592E-3</v>
       </c>
-      <c r="EP15" s="2">
+      <c r="EP15" s="4">
         <v>9.6675838476983705E-4</v>
       </c>
-      <c r="EQ15" s="2">
+      <c r="EQ15" s="4">
         <v>1.7104186807466301E-3</v>
       </c>
-      <c r="ER15" s="2">
+      <c r="ER15" s="4">
         <v>1.5245036067524399E-3</v>
       </c>
-      <c r="ES15" s="2">
+      <c r="ES15" s="4">
         <v>3.30928831709675E-3</v>
       </c>
-      <c r="ET15" s="2">
+      <c r="ET15" s="4">
         <v>1.0411244143675199E-3</v>
       </c>
-      <c r="EU15" s="2">
+      <c r="EU15" s="4">
         <v>1.4873205919535999E-3</v>
       </c>
-      <c r="EV15" s="2">
+      <c r="EV15" s="4">
         <v>1.6360526511489601E-3</v>
       </c>
-      <c r="EW15" s="2">
+      <c r="EW15" s="4">
         <v>2.1937978731315501E-3</v>
       </c>
-      <c r="EX15" s="2">
+      <c r="EX15" s="4">
         <v>2.6399940507176299E-3</v>
       </c>
-      <c r="EY15" s="2">
+      <c r="EY15" s="4">
         <v>1.6732356659478001E-3</v>
       </c>
-      <c r="EZ15" s="2">
+      <c r="EZ15" s="4">
         <v>1.2270394883617201E-3</v>
       </c>
-      <c r="FA15" s="2">
-        <v>0</v>
-      </c>
-      <c r="FB15" s="2">
+      <c r="FA15" s="4">
+        <v>0</v>
+      </c>
+      <c r="FB15" s="4">
         <v>2.9746411839071899E-4</v>
       </c>
-      <c r="FC15" s="2">
+      <c r="FC15" s="4">
         <v>4.8337919238491901E-4</v>
       </c>
-      <c r="FD15" s="2">
+      <c r="FD15" s="4">
         <v>3.3464713318955897E-4</v>
       </c>
-      <c r="FE15" s="2">
+      <c r="FE15" s="4">
         <v>1.1154904439652E-4</v>
       </c>
-      <c r="FF15" s="2">
+      <c r="FF15" s="4">
         <v>6.3211125158027797E-4</v>
       </c>
-      <c r="FG15" s="2">
+      <c r="FG15" s="4">
         <v>1.37577154755708E-3</v>
       </c>
-      <c r="FH15" s="2">
+      <c r="FH15" s="4">
         <v>1.0783074291663599E-3</v>
       </c>
-      <c r="FI15" s="2">
+      <c r="FI15" s="4">
         <v>3.5323864058897899E-3</v>
       </c>
-      <c r="FJ15" s="2">
+      <c r="FJ15" s="4">
         <v>1.2270394883617201E-3</v>
       </c>
-      <c r="FK15" s="2">
+      <c r="FK15" s="4">
         <v>1.7104186807466301E-3</v>
       </c>
-      <c r="FL15" s="2">
+      <c r="FL15" s="4">
         <v>1.7476016955454701E-3</v>
       </c>
-      <c r="FM15" s="2">
+      <c r="FM15" s="4">
         <v>1.2270394883617201E-3</v>
       </c>
-      <c r="FN15" s="2">
+      <c r="FN15" s="4">
         <v>3.8670335390793499E-3</v>
       </c>
-      <c r="FO15" s="2">
+      <c r="FO15" s="4">
         <v>1.0411244143675199E-3</v>
       </c>
-      <c r="FP15" s="2">
+      <c r="FP15" s="4">
         <v>1.0411244143675199E-3</v>
       </c>
-      <c r="FQ15" s="2">
+      <c r="FQ15" s="4">
         <v>7.80843310775638E-4</v>
       </c>
-      <c r="FR15" s="2">
+      <c r="FR15" s="4">
         <v>1.37577154755708E-3</v>
       </c>
-      <c r="FS15" s="2">
+      <c r="FS15" s="4">
         <v>4.0901316278723899E-4</v>
       </c>
-      <c r="FT15" s="2">
+      <c r="FT15" s="4">
         <v>1.45013757715476E-3</v>
       </c>
-      <c r="FU15" s="2">
+      <c r="FU15" s="4">
         <v>1.37577154755708E-3</v>
       </c>
-      <c r="FV15" s="2">
+      <c r="FV15" s="4">
         <v>6.3211125158027797E-4</v>
       </c>
-      <c r="FW15" s="2">
+      <c r="FW15" s="4">
         <v>3.0490072135048699E-3</v>
       </c>
-      <c r="FX15" s="2">
+      <c r="FX15" s="4">
         <v>3.4952033910909501E-3</v>
       </c>
-      <c r="FY15" s="2">
+      <c r="FY15" s="4">
         <v>8.5520934037331699E-4</v>
       </c>
-      <c r="FZ15" s="2">
+      <c r="FZ15" s="4">
         <v>2.0450658139361901E-3</v>
       </c>
-      <c r="GA15" s="2">
+      <c r="GA15" s="4">
         <v>1.89633375474083E-3</v>
       </c>
-      <c r="GB15" s="2">
+      <c r="GB15" s="4">
         <v>2.6771770655164701E-3</v>
       </c>
-      <c r="GC15" s="2">
+      <c r="GC15" s="4">
         <v>1.3014055179594E-3</v>
       </c>
-      <c r="GD15" s="2">
+      <c r="GD15" s="4">
         <v>2.6399940507176299E-3</v>
       </c>
-      <c r="GE15" s="2">
+      <c r="GE15" s="4">
         <v>7.0647728117795804E-4</v>
       </c>
-      <c r="GF15" s="2">
+      <c r="GF15" s="4">
         <v>3.64393545028631E-3</v>
       </c>
-      <c r="GG15" s="2">
+      <c r="GG15" s="4">
         <v>2.0078827991373499E-3</v>
       </c>
-      <c r="GH15" s="2">
+      <c r="GH15" s="4">
         <v>1.8591507399419899E-4</v>
       </c>
-      <c r="GI15" s="2">
+      <c r="GI15" s="4">
         <v>1.45013757715476E-3</v>
       </c>
-      <c r="GJ15" s="2">
+      <c r="GJ15" s="4">
         <v>1.37577154755708E-3</v>
       </c>
-      <c r="GK15" s="2">
+      <c r="GK15" s="4">
         <v>3.9785825834758697E-3</v>
       </c>
-      <c r="GL15" s="2">
+      <c r="GL15" s="4">
         <v>2.9746411839071899E-4</v>
       </c>
-      <c r="GM15" s="2">
+      <c r="GM15" s="4">
         <v>1.2270394883617201E-3</v>
       </c>
-      <c r="GN15" s="2">
+      <c r="GN15" s="4">
         <v>8.5520934037331699E-4</v>
       </c>
-      <c r="GO15" s="2">
+      <c r="GO15" s="4">
         <v>3.7183014798839901E-4</v>
       </c>
-      <c r="GP15" s="2">
+      <c r="GP15" s="4">
         <v>2.23098088793039E-4</v>
       </c>
-      <c r="GQ15" s="2">
+      <c r="GQ15" s="4">
         <v>3.3464713318955897E-4</v>
       </c>
-      <c r="GR15" s="2">
+      <c r="GR15" s="4">
         <v>2.1194318435338701E-3</v>
       </c>
-      <c r="GS15" s="2">
+      <c r="GS15" s="4">
         <v>2.9746411839071899E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:201" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:201" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="4">
         <v>-2.6123742852954199E-2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <v>-0.76964060707535997</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>-0.69149123499135801</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <v>-0.48390540038368901</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <v>0.37748028795376398</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>-0.89245769694171195</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="4">
         <v>6.4858018466570105E-2</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="4">
         <v>-0.93294404141972598</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="4">
         <v>-1.0935863899278599</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="4">
         <v>-0.48103618949840699</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="4">
         <v>-0.88660443896138297</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="4">
         <v>-0.15817227969782399</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="4">
         <v>-0.108823672457216</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="4">
         <v>-1.17607001245703</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="4">
         <v>-0.79998812159718502</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="4">
         <v>-0.13189129749163001</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="4">
         <v>-0.37394202931020698</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="4">
         <v>-0.37648786229928</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="4">
         <v>0.78509411744466995</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="4">
         <v>-0.51137785103502298</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V16" s="4">
         <v>-0.76165116540503097</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W16" s="4">
         <v>-0.92890966404480901</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16" s="4">
         <v>-0.63652778583937297</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Y16" s="4">
         <v>-3.95420294844121E-2</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="Z16" s="4">
         <v>-0.70131371894313999</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AA16" s="4">
         <v>-0.63840100088610197</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AB16" s="4">
         <v>-0.13600016535873599</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AC16" s="4">
         <v>-0.89676693269260799</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AD16" s="4">
         <v>-1.2046451757376699</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AE16" s="4">
         <v>-0.848877558891726</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="AF16" s="4">
         <v>-0.19293459941932101</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="AG16" s="4">
         <v>-0.66407465393533205</v>
       </c>
-      <c r="AH16" s="2">
+      <c r="AH16" s="4">
         <v>-0.81965716121012999</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AI16" s="4">
         <v>0.47550493283649398</v>
       </c>
-      <c r="AJ16" s="2">
+      <c r="AJ16" s="4">
         <v>-0.210603779063328</v>
       </c>
-      <c r="AK16" s="2">
+      <c r="AK16" s="4">
         <v>-0.86841172172575298</v>
       </c>
-      <c r="AL16" s="2">
+      <c r="AL16" s="4">
         <v>-1.0218781121398199</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="AM16" s="4">
         <v>-1.01737077647411</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="AN16" s="4">
         <v>-0.37134177037025001</v>
       </c>
-      <c r="AO16" s="2">
+      <c r="AO16" s="4">
         <v>-0.92698720936050905</v>
       </c>
-      <c r="AP16" s="2">
+      <c r="AP16" s="4">
         <v>-0.31598934351489699</v>
       </c>
-      <c r="AQ16" s="2">
+      <c r="AQ16" s="4">
         <v>-0.94033138671957495</v>
       </c>
-      <c r="AR16" s="2">
+      <c r="AR16" s="4">
         <v>0.90710873468982001</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AS16" s="4">
         <v>-0.106854707191292</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AT16" s="4">
         <v>-0.81540448650756703</v>
       </c>
-      <c r="AU16" s="2">
+      <c r="AU16" s="4">
         <v>-0.83535656409631798</v>
       </c>
-      <c r="AV16" s="2">
+      <c r="AV16" s="4">
         <v>-0.50700893885390097</v>
       </c>
-      <c r="AW16" s="2">
+      <c r="AW16" s="4">
         <v>-0.43479265697035102</v>
       </c>
-      <c r="AX16" s="2">
+      <c r="AX16" s="4">
         <v>-4.2221090435267498E-2</v>
       </c>
-      <c r="AY16" s="2">
+      <c r="AY16" s="4">
         <v>-0.51995966108129998</v>
       </c>
-      <c r="AZ16" s="2">
+      <c r="AZ16" s="4">
         <v>-0.91254759030240296</v>
       </c>
-      <c r="BA16" s="2">
+      <c r="BA16" s="4">
         <v>0.41952830169821298</v>
       </c>
-      <c r="BB16" s="2">
+      <c r="BB16" s="4">
         <v>0.77441550227039402</v>
       </c>
-      <c r="BC16" s="2">
+      <c r="BC16" s="4">
         <v>-0.81963583551113695</v>
       </c>
-      <c r="BD16" s="2">
+      <c r="BD16" s="4">
         <v>-0.80633507293406603</v>
       </c>
-      <c r="BE16" s="2">
+      <c r="BE16" s="4">
         <v>-0.77115094175119303</v>
       </c>
-      <c r="BF16" s="2">
+      <c r="BF16" s="4">
         <v>-1.1696220821005401</v>
       </c>
-      <c r="BG16" s="2">
+      <c r="BG16" s="4">
         <v>0.13571153549509701</v>
       </c>
-      <c r="BH16" s="2">
+      <c r="BH16" s="4">
         <v>-3.3410637426126003E-2</v>
       </c>
-      <c r="BI16" s="2">
+      <c r="BI16" s="4">
         <v>0.75291114927239</v>
       </c>
-      <c r="BJ16" s="2">
+      <c r="BJ16" s="4">
         <v>-0.48237017421723999</v>
       </c>
-      <c r="BK16" s="2">
+      <c r="BK16" s="4">
         <v>0.78497951804978205</v>
       </c>
-      <c r="BL16" s="2">
+      <c r="BL16" s="4">
         <v>0.70178676039642995</v>
       </c>
-      <c r="BM16" s="2">
+      <c r="BM16" s="4">
         <v>-0.92444910723615104</v>
       </c>
-      <c r="BN16" s="2">
+      <c r="BN16" s="4">
         <v>3.5671342045147297E-2</v>
       </c>
-      <c r="BO16" s="2">
+      <c r="BO16" s="4">
         <v>-1.13930132484544</v>
       </c>
-      <c r="BP16" s="2">
+      <c r="BP16" s="4">
         <v>-0.12104966952379501</v>
       </c>
-      <c r="BQ16" s="2">
+      <c r="BQ16" s="4">
         <v>0.159210431475236</v>
       </c>
-      <c r="BR16" s="2">
+      <c r="BR16" s="4">
         <v>0.69247785041871501</v>
       </c>
-      <c r="BS16" s="2">
+      <c r="BS16" s="4">
         <v>-0.65652650016149405</v>
       </c>
-      <c r="BT16" s="2">
+      <c r="BT16" s="4">
         <v>-0.78659158741885304</v>
       </c>
-      <c r="BU16" s="2">
+      <c r="BU16" s="4">
         <v>-1.04960633713386</v>
       </c>
-      <c r="BV16" s="2">
+      <c r="BV16" s="4">
         <v>1.76364285487142</v>
       </c>
-      <c r="BW16" s="2">
+      <c r="BW16" s="4">
         <v>-0.61244359414913696</v>
       </c>
-      <c r="BX16" s="2">
+      <c r="BX16" s="4">
         <v>1.4560623633548</v>
       </c>
-      <c r="BY16" s="2">
+      <c r="BY16" s="4">
         <v>1.9447368007857999E-2</v>
       </c>
-      <c r="BZ16" s="2">
+      <c r="BZ16" s="4">
         <v>0.50445332892021999</v>
       </c>
-      <c r="CA16" s="2">
+      <c r="CA16" s="4">
         <v>0.76295986908611901</v>
       </c>
-      <c r="CB16" s="2">
+      <c r="CB16" s="4">
         <v>0.62290649538461695</v>
       </c>
-      <c r="CC16" s="2">
+      <c r="CC16" s="4">
         <v>-1.18396831170266</v>
       </c>
-      <c r="CD16" s="2">
+      <c r="CD16" s="4">
         <v>-1.0383336989373</v>
       </c>
-      <c r="CE16" s="2">
+      <c r="CE16" s="4">
         <v>-0.76445058063343096</v>
       </c>
-      <c r="CF16" s="2">
+      <c r="CF16" s="4">
         <v>-0.704123347086272</v>
       </c>
-      <c r="CG16" s="2">
+      <c r="CG16" s="4">
         <v>-0.38626067229859701</v>
       </c>
-      <c r="CH16" s="2">
+      <c r="CH16" s="4">
         <v>-0.83792913241520195</v>
       </c>
-      <c r="CI16" s="2">
+      <c r="CI16" s="4">
         <v>-1.2263476959876601E-2</v>
       </c>
-      <c r="CJ16" s="2">
+      <c r="CJ16" s="4">
         <v>-0.15923544645993901</v>
       </c>
-      <c r="CK16" s="2">
+      <c r="CK16" s="4">
         <v>0.32922205146413602</v>
       </c>
-      <c r="CL16" s="2">
+      <c r="CL16" s="4">
         <v>0.209970508603499</v>
       </c>
-      <c r="CM16" s="2">
+      <c r="CM16" s="4">
         <v>-0.82014286316482399</v>
       </c>
-      <c r="CN16" s="2">
+      <c r="CN16" s="4">
         <v>1.2105547663793099</v>
       </c>
-      <c r="CO16" s="2">
+      <c r="CO16" s="4">
         <v>-0.97961758361818296</v>
       </c>
-      <c r="CP16" s="2">
+      <c r="CP16" s="4">
         <v>0.58973005088973596</v>
       </c>
-      <c r="CQ16" s="2">
+      <c r="CQ16" s="4">
         <v>0.239402706261482</v>
       </c>
-      <c r="CR16" s="2">
+      <c r="CR16" s="4">
         <v>0.866835001505733</v>
       </c>
-      <c r="CS16" s="2">
+      <c r="CS16" s="4">
         <v>-1.2119056600521401</v>
       </c>
-      <c r="CT16" s="2">
+      <c r="CT16" s="4">
         <v>0.73764373503532599</v>
       </c>
-      <c r="CU16" s="2">
+      <c r="CU16" s="4">
         <v>-1.0458571559307499</v>
       </c>
-      <c r="CV16" s="2">
+      <c r="CV16" s="4">
         <v>1.28746733042992</v>
       </c>
-      <c r="CW16" s="2">
+      <c r="CW16" s="4">
         <v>1.20647935854413</v>
       </c>
-      <c r="CX16" s="2">
+      <c r="CX16" s="4">
         <v>3.6845907730415899E-2</v>
       </c>
-      <c r="CY16" s="2">
+      <c r="CY16" s="4">
         <v>2.6782949736814901E-2</v>
       </c>
-      <c r="CZ16" s="2">
+      <c r="CZ16" s="4">
         <v>2.8795541335535101E-2</v>
       </c>
-      <c r="DA16" s="2">
+      <c r="DA16" s="4">
         <v>1.48622148828568E-2</v>
       </c>
-      <c r="DB16" s="2">
+      <c r="DB16" s="4">
         <v>7.8955516565177002E-3</v>
       </c>
-      <c r="DC16" s="2">
+      <c r="DC16" s="4">
         <v>1.29012281969243E-2</v>
       </c>
-      <c r="DD16" s="2">
+      <c r="DD16" s="4">
         <v>1.1249870987718E-2</v>
       </c>
-      <c r="DE16" s="2">
+      <c r="DE16" s="4">
         <v>6.0893797089482896E-3</v>
       </c>
-      <c r="DF16" s="2">
+      <c r="DF16" s="4">
         <v>1.11466611621426E-2</v>
       </c>
-      <c r="DG16" s="2">
+      <c r="DG16" s="4">
         <v>4.3864175869542804E-3</v>
       </c>
-      <c r="DH16" s="2">
+      <c r="DH16" s="4">
         <v>5.0056765404066497E-3</v>
       </c>
-      <c r="DI16" s="2">
+      <c r="DI16" s="4">
         <v>4.6444421508927596E-3</v>
       </c>
-      <c r="DJ16" s="2">
+      <c r="DJ16" s="4">
         <v>7.3278976158530299E-3</v>
       </c>
-      <c r="DK16" s="2">
+      <c r="DK16" s="4">
         <v>5.6765404066467101E-3</v>
       </c>
-      <c r="DL16" s="2">
+      <c r="DL16" s="4">
         <v>4.5412323253173703E-3</v>
       </c>
-      <c r="DM16" s="2">
+      <c r="DM16" s="4">
         <v>5.4185158427082301E-3</v>
       </c>
-      <c r="DN16" s="2">
+      <c r="DN16" s="4">
         <v>1.65135720920632E-3</v>
       </c>
-      <c r="DO16" s="2">
+      <c r="DO16" s="4">
         <v>1.39333264526783E-3</v>
       </c>
-      <c r="DP16" s="2">
+      <c r="DP16" s="4">
         <v>4.8508618020435502E-3</v>
       </c>
-      <c r="DQ16" s="2">
+      <c r="DQ16" s="4">
         <v>1.65135720920632E-3</v>
       </c>
-      <c r="DR16" s="2">
+      <c r="DR16" s="4">
         <v>3.5091340695634198E-3</v>
       </c>
-      <c r="DS16" s="2">
+      <c r="DS16" s="4">
         <v>4.4896274125296697E-3</v>
       </c>
-      <c r="DT16" s="2">
+      <c r="DT16" s="4">
         <v>1.34172773248013E-3</v>
       </c>
-      <c r="DU16" s="2">
+      <c r="DU16" s="4">
         <v>2.8382702033233598E-3</v>
       </c>
-      <c r="DV16" s="2">
+      <c r="DV16" s="4">
         <v>5.05728145319434E-3</v>
       </c>
-      <c r="DW16" s="2">
+      <c r="DW16" s="4">
         <v>2.52864072659717E-3</v>
       </c>
-      <c r="DX16" s="2">
+      <c r="DX16" s="4">
         <v>2.4770358138094702E-3</v>
       </c>
-      <c r="DY16" s="2">
+      <c r="DY16" s="4">
         <v>2.9414800288987499E-3</v>
       </c>
-      <c r="DZ16" s="2">
+      <c r="DZ16" s="4">
         <v>1.0320982557539501E-3</v>
       </c>
-      <c r="EA16" s="2">
+      <c r="EA16" s="4">
         <v>1.5481473836309199E-3</v>
       </c>
-      <c r="EB16" s="2">
+      <c r="EB16" s="4">
         <v>4.12839302301579E-3</v>
       </c>
-      <c r="EC16" s="2">
+      <c r="EC16" s="4">
         <v>4.0251831974403999E-3</v>
       </c>
-      <c r="ED16" s="2">
+      <c r="ED16" s="4">
         <v>2.52864072659717E-3</v>
       </c>
-      <c r="EE16" s="2">
+      <c r="EE16" s="4">
         <v>2.5802456393848698E-3</v>
       </c>
-      <c r="EF16" s="2">
+      <c r="EF16" s="4">
         <v>1.4965424708432199E-3</v>
       </c>
-      <c r="EG16" s="2">
+      <c r="EG16" s="4">
         <v>3.4059242439880301E-3</v>
       </c>
-      <c r="EH16" s="2">
+      <c r="EH16" s="4">
         <v>4.1283930230157897E-4</v>
       </c>
-      <c r="EI16" s="2">
+      <c r="EI16" s="4">
         <v>1.0837031685416499E-3</v>
       </c>
-      <c r="EJ16" s="2">
+      <c r="EJ16" s="4">
         <v>3.0962947672618399E-4</v>
       </c>
-      <c r="EK16" s="2">
+      <c r="EK16" s="4">
         <v>2.3222210754463798E-3</v>
       </c>
-      <c r="EL16" s="2">
+      <c r="EL16" s="4">
         <v>9.8049334296625005E-4</v>
       </c>
-      <c r="EM16" s="2">
+      <c r="EM16" s="4">
         <v>3.3543193312003299E-3</v>
       </c>
-      <c r="EN16" s="2">
+      <c r="EN16" s="4">
         <v>8.2567860460315795E-4</v>
       </c>
-      <c r="EO16" s="2">
+      <c r="EO16" s="4">
         <v>8.2567860460315795E-4</v>
       </c>
-      <c r="EP16" s="2">
+      <c r="EP16" s="4">
         <v>2.0641965115079E-4</v>
       </c>
-      <c r="EQ16" s="2">
+      <c r="EQ16" s="4">
         <v>2.0125915987201999E-3</v>
       </c>
-      <c r="ER16" s="2">
+      <c r="ER16" s="4">
         <v>1.18691299411704E-3</v>
       </c>
-      <c r="ES16" s="2">
+      <c r="ES16" s="4">
         <v>3.9219733718650002E-3</v>
       </c>
-      <c r="ET16" s="2">
+      <c r="ET16" s="4">
         <v>6.7086386624006596E-4</v>
       </c>
-      <c r="EU16" s="2">
+      <c r="EU16" s="4">
         <v>6.1925895345236895E-4</v>
       </c>
-      <c r="EV16" s="2">
+      <c r="EV16" s="4">
         <v>2.3222210754463798E-3</v>
       </c>
-      <c r="EW16" s="2">
+      <c r="EW16" s="4">
         <v>3.9735782846527E-3</v>
       </c>
-      <c r="EX16" s="2">
+      <c r="EX16" s="4">
         <v>1.65135720920632E-3</v>
       </c>
-      <c r="EY16" s="2">
+      <c r="EY16" s="4">
         <v>3.1478996800495401E-3</v>
       </c>
-      <c r="EZ16" s="2">
+      <c r="EZ16" s="4">
         <v>1.0837031685416499E-3</v>
       </c>
-      <c r="FA16" s="2">
-        <v>0</v>
-      </c>
-      <c r="FB16" s="2">
+      <c r="FA16" s="4">
+        <v>0</v>
+      </c>
+      <c r="FB16" s="4">
         <v>4.1283930230157897E-4</v>
       </c>
-      <c r="FC16" s="2">
+      <c r="FC16" s="4">
         <v>3.0962947672618399E-4</v>
       </c>
-      <c r="FD16" s="2">
+      <c r="FD16" s="4">
         <v>2.5802456393848698E-4</v>
       </c>
-      <c r="FE16" s="2">
+      <c r="FE16" s="4">
         <v>1.03209825575395E-4</v>
       </c>
-      <c r="FF16" s="2">
+      <c r="FF16" s="4">
         <v>5.6765404066467097E-4</v>
       </c>
-      <c r="FG16" s="2">
+      <c r="FG16" s="4">
         <v>6.1925895345236895E-4</v>
       </c>
-      <c r="FH16" s="2">
+      <c r="FH16" s="4">
         <v>1.7545670347817099E-3</v>
       </c>
-      <c r="FI16" s="2">
+      <c r="FI16" s="4">
         <v>1.80617194756941E-3</v>
       </c>
-      <c r="FJ16" s="2">
+      <c r="FJ16" s="4">
         <v>8.2567860460315795E-4</v>
       </c>
-      <c r="FK16" s="2">
+      <c r="FK16" s="4">
         <v>1.39333264526783E-3</v>
       </c>
-      <c r="FL16" s="2">
+      <c r="FL16" s="4">
         <v>1.44493755805553E-3</v>
       </c>
-      <c r="FM16" s="2">
+      <c r="FM16" s="4">
         <v>1.34172773248013E-3</v>
       </c>
-      <c r="FN16" s="2">
+      <c r="FN16" s="4">
         <v>3.0962947672618399E-3</v>
       </c>
-      <c r="FO16" s="2">
+      <c r="FO16" s="4">
         <v>1.2385179069047401E-3</v>
       </c>
-      <c r="FP16" s="2">
+      <c r="FP16" s="4">
         <v>1.34172773248013E-3</v>
       </c>
-      <c r="FQ16" s="2">
+      <c r="FQ16" s="4">
         <v>6.1925895345236895E-4</v>
       </c>
-      <c r="FR16" s="2">
+      <c r="FR16" s="4">
         <v>1.13530808132934E-3</v>
       </c>
-      <c r="FS16" s="2">
+      <c r="FS16" s="4">
         <v>6.7086386624006596E-4</v>
       </c>
-      <c r="FT16" s="2">
+      <c r="FT16" s="4">
         <v>1.9093817731448001E-3</v>
       </c>
-      <c r="FU16" s="2">
+      <c r="FU16" s="4">
         <v>2.0641965115079002E-3</v>
       </c>
-      <c r="FV16" s="2">
+      <c r="FV16" s="4">
         <v>8.2567860460315795E-4</v>
       </c>
-      <c r="FW16" s="2">
+      <c r="FW16" s="4">
         <v>1.80617194756941E-3</v>
       </c>
-      <c r="FX16" s="2">
+      <c r="FX16" s="4">
         <v>9.8049334296625005E-4</v>
       </c>
-      <c r="FY16" s="2">
+      <c r="FY16" s="4">
         <v>7.7407369181546105E-4</v>
       </c>
-      <c r="FZ16" s="2">
+      <c r="FZ16" s="4">
         <v>1.59975229641862E-3</v>
       </c>
-      <c r="GA16" s="2">
+      <c r="GA16" s="4">
         <v>8.2567860460315795E-4</v>
       </c>
-      <c r="GB16" s="2">
+      <c r="GB16" s="4">
         <v>1.65135720920632E-3</v>
       </c>
-      <c r="GC16" s="2">
+      <c r="GC16" s="4">
         <v>8.7728351739085604E-4</v>
       </c>
-      <c r="GD16" s="2">
+      <c r="GD16" s="4">
         <v>1.59975229641862E-3</v>
       </c>
-      <c r="GE16" s="2">
+      <c r="GE16" s="4">
         <v>6.1925895345236895E-4</v>
       </c>
-      <c r="GF16" s="2">
+      <c r="GF16" s="4">
         <v>1.9093817731448001E-3</v>
       </c>
-      <c r="GG16" s="2">
+      <c r="GG16" s="4">
         <v>1.7029621219940101E-3</v>
       </c>
-      <c r="GH16" s="2">
-        <v>0</v>
-      </c>
-      <c r="GI16" s="2">
+      <c r="GH16" s="4">
+        <v>0</v>
+      </c>
+      <c r="GI16" s="4">
         <v>6.1925895345236895E-4</v>
       </c>
-      <c r="GJ16" s="2">
+      <c r="GJ16" s="4">
         <v>1.2385179069047401E-3</v>
       </c>
-      <c r="GK16" s="2">
+      <c r="GK16" s="4">
         <v>1.5481473836309199E-3</v>
       </c>
-      <c r="GL16" s="2">
+      <c r="GL16" s="4">
         <v>9.2888843017855304E-4</v>
       </c>
-      <c r="GM16" s="2">
+      <c r="GM16" s="4">
         <v>1.4965424708432199E-3</v>
       </c>
-      <c r="GN16" s="2">
+      <c r="GN16" s="4">
         <v>3.6123438951388202E-4</v>
       </c>
-      <c r="GO16" s="2">
+      <c r="GO16" s="4">
         <v>5.1604912787697396E-4</v>
       </c>
-      <c r="GP16" s="2">
+      <c r="GP16" s="4">
         <v>1.03209825575395E-4</v>
       </c>
-      <c r="GQ16" s="2">
+      <c r="GQ16" s="4">
         <v>3.6123438951388202E-4</v>
       </c>
-      <c r="GR16" s="2">
+      <c r="GR16" s="4">
         <v>2.2190112498709901E-3</v>
       </c>
-      <c r="GS16" s="2">
+      <c r="GS16" s="4">
         <v>6.7086386624006596E-4</v>
       </c>
     </row>
@@ -75242,6 +75242,12 @@
       <c r="CW24">
         <f t="shared" si="4"/>
         <v>5.4825391412149926E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:201" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>AVERAGE(B24:Y24)</f>
+        <v>1.0235324674247275</v>
       </c>
     </row>
   </sheetData>
@@ -75249,18 +75255,19 @@
     <sortCondition descending="1" ref="B24:CW24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CW24"/>
+  <dimension ref="A1:CW26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -81240,6 +81247,12 @@
       <c r="CW24">
         <f t="shared" si="2"/>
         <v>1.9661237498035999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>AVERAGE(B24:Y24)</f>
+        <v>1.119352257388923</v>
       </c>
     </row>
   </sheetData>
@@ -81252,13 +81265,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CW24"/>
+  <dimension ref="A1:CW26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -86840,404 +86853,410 @@
         <v>567</v>
       </c>
       <c r="B24">
-        <f>ABS(B15-B16)</f>
+        <f t="shared" ref="B24:AG24" si="0">ABS(B15-B16)</f>
         <v>2.381733161339239</v>
       </c>
       <c r="C24">
-        <f>ABS(C15-C16)</f>
+        <f t="shared" si="0"/>
         <v>2.2517130123429503</v>
       </c>
       <c r="D24">
-        <f>ABS(D15-D16)</f>
+        <f t="shared" si="0"/>
         <v>2.1765803717792602</v>
       </c>
       <c r="E24">
-        <f>ABS(E15-E16)</f>
+        <f t="shared" si="0"/>
         <v>1.9397524970363971</v>
       </c>
       <c r="F24">
-        <f>ABS(F15-F16)</f>
+        <f t="shared" si="0"/>
         <v>1.87665600942608</v>
       </c>
       <c r="G24">
-        <f>ABS(G15-G16)</f>
+        <f t="shared" si="0"/>
         <v>1.8705351908208041</v>
       </c>
       <c r="H24">
-        <f>ABS(H15-H16)</f>
+        <f t="shared" si="0"/>
         <v>1.6081485522504311</v>
       </c>
       <c r="I24">
-        <f>ABS(I15-I16)</f>
+        <f t="shared" si="0"/>
         <v>1.5950573309236871</v>
       </c>
       <c r="J24">
-        <f>ABS(J15-J16)</f>
+        <f t="shared" si="0"/>
         <v>1.57921636095699</v>
       </c>
       <c r="K24">
-        <f>ABS(K15-K16)</f>
+        <f t="shared" si="0"/>
         <v>1.5591360629566642</v>
       </c>
       <c r="L24">
-        <f>ABS(L15-L16)</f>
+        <f t="shared" si="0"/>
         <v>1.4526577506996421</v>
       </c>
       <c r="M24">
-        <f>ABS(M15-M16)</f>
+        <f t="shared" si="0"/>
         <v>1.388502094253113</v>
       </c>
       <c r="N24">
-        <f>ABS(N15-N16)</f>
+        <f t="shared" si="0"/>
         <v>1.3403053170690351</v>
       </c>
       <c r="O24">
-        <f>ABS(O15-O16)</f>
+        <f t="shared" si="0"/>
         <v>1.3216678285385339</v>
       </c>
       <c r="P24">
-        <f>ABS(P15-P16)</f>
+        <f t="shared" si="0"/>
         <v>1.1800397640655729</v>
       </c>
       <c r="Q24">
-        <f>ABS(Q15-Q16)</f>
+        <f t="shared" si="0"/>
         <v>1.1764600289816114</v>
       </c>
       <c r="R24">
-        <f>ABS(R15-R16)</f>
+        <f t="shared" si="0"/>
         <v>1.1260679348321421</v>
       </c>
       <c r="S24">
-        <f>ABS(S15-S16)</f>
+        <f t="shared" si="0"/>
         <v>1.0396266518845652</v>
       </c>
       <c r="T24">
-        <f>ABS(T15-T16)</f>
+        <f t="shared" si="0"/>
         <v>1.0159757148723969</v>
       </c>
       <c r="U24">
-        <f>ABS(U15-U16)</f>
+        <f t="shared" si="0"/>
         <v>0.93363429104279005</v>
       </c>
       <c r="V24">
-        <f>ABS(V15-V16)</f>
+        <f t="shared" si="0"/>
         <v>0.92794924097264397</v>
       </c>
       <c r="W24">
-        <f>ABS(W15-W16)</f>
+        <f t="shared" si="0"/>
         <v>0.86952995808827804</v>
       </c>
       <c r="X24">
-        <f>ABS(X15-X16)</f>
+        <f t="shared" si="0"/>
         <v>0.82893755465556906</v>
       </c>
       <c r="Y24">
-        <f>ABS(Y15-Y16)</f>
+        <f t="shared" si="0"/>
         <v>0.76064824401795894</v>
       </c>
       <c r="Z24">
-        <f>ABS(Z15-Z16)</f>
+        <f t="shared" si="0"/>
         <v>0.73553306798636398</v>
       </c>
       <c r="AA24">
-        <f>ABS(AA15-AA16)</f>
+        <f t="shared" si="0"/>
         <v>0.73332341050818406</v>
       </c>
       <c r="AB24">
-        <f>ABS(AB15-AB16)</f>
+        <f t="shared" si="0"/>
         <v>0.71538027647113001</v>
       </c>
       <c r="AC24">
-        <f>ABS(AC15-AC16)</f>
+        <f t="shared" si="0"/>
         <v>0.69266019449916272</v>
       </c>
       <c r="AD24">
-        <f>ABS(AD15-AD16)</f>
+        <f t="shared" si="0"/>
         <v>0.67502737600042706</v>
       </c>
       <c r="AE24">
-        <f>ABS(AE15-AE16)</f>
+        <f t="shared" si="0"/>
         <v>0.6615563746036599</v>
       </c>
       <c r="AF24">
-        <f>ABS(AF15-AF16)</f>
+        <f t="shared" si="0"/>
         <v>0.64988635846644094</v>
       </c>
       <c r="AG24">
-        <f>ABS(AG15-AG16)</f>
+        <f t="shared" si="0"/>
         <v>0.60900598001475204</v>
       </c>
       <c r="AH24">
-        <f>ABS(AH15-AH16)</f>
+        <f t="shared" ref="AH24:BM24" si="1">ABS(AH15-AH16)</f>
         <v>0.59034834652095691</v>
       </c>
       <c r="AI24">
-        <f>ABS(AI15-AI16)</f>
+        <f t="shared" si="1"/>
         <v>0.58024120041946592</v>
       </c>
       <c r="AJ24">
-        <f>ABS(AJ15-AJ16)</f>
+        <f t="shared" si="1"/>
         <v>0.55620368417528898</v>
       </c>
       <c r="AK24">
-        <f>ABS(AK15-AK16)</f>
+        <f t="shared" si="1"/>
         <v>0.55557077355288398</v>
       </c>
       <c r="AL24">
-        <f>ABS(AL15-AL16)</f>
+        <f t="shared" si="1"/>
         <v>0.55279368325274103</v>
       </c>
       <c r="AM24">
-        <f>ABS(AM15-AM16)</f>
+        <f t="shared" si="1"/>
         <v>0.5228214897363499</v>
       </c>
       <c r="AN24">
-        <f>ABS(AN15-AN16)</f>
+        <f t="shared" si="1"/>
         <v>0.48774858158920587</v>
       </c>
       <c r="AO24">
-        <f>ABS(AO15-AO16)</f>
+        <f t="shared" si="1"/>
         <v>0.46601973593065993</v>
       </c>
       <c r="AP24">
-        <f>ABS(AP15-AP16)</f>
+        <f t="shared" si="1"/>
         <v>0.44324065404832402</v>
       </c>
       <c r="AQ24">
-        <f>ABS(AQ15-AQ16)</f>
+        <f t="shared" si="1"/>
         <v>0.42717223957503192</v>
       </c>
       <c r="AR24">
-        <f>ABS(AR15-AR16)</f>
+        <f t="shared" si="1"/>
         <v>0.40646442749467104</v>
       </c>
       <c r="AS24">
-        <f>ABS(AS15-AS16)</f>
+        <f t="shared" si="1"/>
         <v>0.39829898364744099</v>
       </c>
       <c r="AT24">
-        <f>ABS(AT15-AT16)</f>
+        <f t="shared" si="1"/>
         <v>0.39803100174292105</v>
       </c>
       <c r="AU24">
-        <f>ABS(AU15-AU16)</f>
+        <f t="shared" si="1"/>
         <v>0.38375086979183104</v>
       </c>
       <c r="AV24">
-        <f>ABS(AV15-AV16)</f>
+        <f t="shared" si="1"/>
         <v>0.37780168676133608</v>
       </c>
       <c r="AW24">
-        <f>ABS(AW15-AW16)</f>
+        <f t="shared" si="1"/>
         <v>0.36300164281272707</v>
       </c>
       <c r="AX24">
-        <f>ABS(AX15-AX16)</f>
+        <f t="shared" si="1"/>
         <v>0.3613038835167901</v>
       </c>
       <c r="AY24">
-        <f>ABS(AY15-AY16)</f>
+        <f t="shared" si="1"/>
         <v>0.35562391419778205</v>
       </c>
       <c r="AZ24">
-        <f>ABS(AZ15-AZ16)</f>
+        <f t="shared" si="1"/>
         <v>0.34842889317594095</v>
       </c>
       <c r="BA24">
-        <f>ABS(BA15-BA16)</f>
+        <f t="shared" si="1"/>
         <v>0.33846536588215281</v>
       </c>
       <c r="BB24">
-        <f>ABS(BB15-BB16)</f>
+        <f t="shared" si="1"/>
         <v>0.31965720403851361</v>
       </c>
       <c r="BC24">
-        <f>ABS(BC15-BC16)</f>
+        <f t="shared" si="1"/>
         <v>0.318049520998614</v>
       </c>
       <c r="BD24">
-        <f>ABS(BD15-BD16)</f>
+        <f t="shared" si="1"/>
         <v>0.30340586863728591</v>
       </c>
       <c r="BE24">
-        <f>ABS(BE15-BE16)</f>
+        <f t="shared" si="1"/>
         <v>0.30064837674820699</v>
       </c>
       <c r="BF24">
-        <f>ABS(BF15-BF16)</f>
+        <f t="shared" si="1"/>
         <v>0.298448932071818</v>
       </c>
       <c r="BG24">
-        <f>ABS(BG15-BG16)</f>
+        <f t="shared" si="1"/>
         <v>0.28972728213801702</v>
       </c>
       <c r="BH24">
-        <f>ABS(BH15-BH16)</f>
+        <f t="shared" si="1"/>
         <v>0.28577662390106295</v>
       </c>
       <c r="BI24">
-        <f>ABS(BI15-BI16)</f>
+        <f t="shared" si="1"/>
         <v>0.26336617544234575</v>
       </c>
       <c r="BJ24">
-        <f>ABS(BJ15-BJ16)</f>
+        <f t="shared" si="1"/>
         <v>0.25921557979092802</v>
       </c>
       <c r="BK24">
-        <f>ABS(BK15-BK16)</f>
+        <f t="shared" si="1"/>
         <v>0.24982708992053893</v>
       </c>
       <c r="BL24">
-        <f>ABS(BL15-BL16)</f>
+        <f t="shared" si="1"/>
         <v>0.23417762860776803</v>
       </c>
       <c r="BM24">
-        <f>ABS(BM15-BM16)</f>
+        <f t="shared" si="1"/>
         <v>0.216251708885976</v>
       </c>
       <c r="BN24">
-        <f>ABS(BN15-BN16)</f>
+        <f t="shared" ref="BN24:CW24" si="2">ABS(BN15-BN16)</f>
         <v>0.21567580381840101</v>
       </c>
       <c r="BO24">
-        <f>ABS(BO15-BO16)</f>
+        <f t="shared" si="2"/>
         <v>0.20608327229682599</v>
       </c>
       <c r="BP24">
-        <f>ABS(BP15-BP16)</f>
+        <f t="shared" si="2"/>
         <v>0.20486195733896201</v>
       </c>
       <c r="BQ24">
-        <f>ABS(BQ15-BQ16)</f>
+        <f t="shared" si="2"/>
         <v>0.19760520905389639</v>
       </c>
       <c r="BR24">
-        <f>ABS(BR15-BR16)</f>
+        <f t="shared" si="2"/>
         <v>0.18063300884964706</v>
       </c>
       <c r="BS24">
-        <f>ABS(BS15-BS16)</f>
+        <f t="shared" si="2"/>
         <v>0.15540541197618007</v>
       </c>
       <c r="BT24">
-        <f>ABS(BT15-BT16)</f>
+        <f t="shared" si="2"/>
         <v>0.15449719038919008</v>
       </c>
       <c r="BU24">
-        <f>ABS(BU15-BU16)</f>
+        <f t="shared" si="2"/>
         <v>0.15256884180977193</v>
       </c>
       <c r="BV24">
-        <f>ABS(BV15-BV16)</f>
+        <f t="shared" si="2"/>
         <v>0.1515210125107519</v>
       </c>
       <c r="BW24">
-        <f>ABS(BW15-BW16)</f>
+        <f t="shared" si="2"/>
         <v>0.14944729438721202</v>
       </c>
       <c r="BX24">
-        <f>ABS(BX15-BX16)</f>
+        <f t="shared" si="2"/>
         <v>0.13855268495120299</v>
       </c>
       <c r="BY24">
-        <f>ABS(BY15-BY16)</f>
+        <f t="shared" si="2"/>
         <v>0.13815363897240907</v>
       </c>
       <c r="BZ24">
-        <f>ABS(BZ15-BZ16)</f>
+        <f t="shared" si="2"/>
         <v>0.12048840322648791</v>
       </c>
       <c r="CA24">
-        <f>ABS(CA15-CA16)</f>
+        <f t="shared" si="2"/>
         <v>0.11944785016658499</v>
       </c>
       <c r="CB24">
-        <f>ABS(CB15-CB16)</f>
+        <f t="shared" si="2"/>
         <v>0.11363450213232595</v>
       </c>
       <c r="CC24">
-        <f>ABS(CC15-CC16)</f>
+        <f t="shared" si="2"/>
         <v>0.107813947106907</v>
       </c>
       <c r="CD24">
-        <f>ABS(CD15-CD16)</f>
+        <f t="shared" si="2"/>
         <v>0.10716130841796701</v>
       </c>
       <c r="CE24">
-        <f>ABS(CE15-CE16)</f>
+        <f t="shared" si="2"/>
         <v>0.10543317722304096</v>
       </c>
       <c r="CF24">
-        <f>ABS(CF15-CF16)</f>
+        <f t="shared" si="2"/>
         <v>9.4518126722919038E-2</v>
       </c>
       <c r="CG24">
-        <f>ABS(CG15-CG16)</f>
+        <f t="shared" si="2"/>
         <v>9.2009538131510027E-2</v>
       </c>
       <c r="CH24">
-        <f>ABS(CH15-CH16)</f>
+        <f t="shared" si="2"/>
         <v>8.6264828639888935E-2</v>
       </c>
       <c r="CI24">
-        <f>ABS(CI15-CI16)</f>
+        <f t="shared" si="2"/>
         <v>7.5280574893985985E-2</v>
       </c>
       <c r="CJ24">
-        <f>ABS(CJ15-CJ16)</f>
+        <f t="shared" si="2"/>
         <v>7.3787100210089496E-2</v>
       </c>
       <c r="CK24">
-        <f>ABS(CK15-CK16)</f>
+        <f t="shared" si="2"/>
         <v>7.3111659523993011E-2</v>
       </c>
       <c r="CL24">
-        <f>ABS(CL15-CL16)</f>
+        <f t="shared" si="2"/>
         <v>6.1944137081790029E-2</v>
       </c>
       <c r="CM24">
-        <f>ABS(CM15-CM16)</f>
+        <f t="shared" si="2"/>
         <v>5.5749714683535956E-2</v>
       </c>
       <c r="CN24">
-        <f>ABS(CN15-CN16)</f>
+        <f t="shared" si="2"/>
         <v>4.3161580115996023E-2</v>
       </c>
       <c r="CO24">
-        <f>ABS(CO15-CO16)</f>
+        <f t="shared" si="2"/>
         <v>3.6290578052074918E-2</v>
       </c>
       <c r="CP24">
-        <f>ABS(CP15-CP16)</f>
+        <f t="shared" si="2"/>
         <v>2.4318412473790074E-2</v>
       </c>
       <c r="CQ24">
-        <f>ABS(CQ15-CQ16)</f>
+        <f t="shared" si="2"/>
         <v>2.2294459632252017E-2</v>
       </c>
       <c r="CR24">
-        <f>ABS(CR15-CR16)</f>
+        <f t="shared" si="2"/>
         <v>1.8879088896279983E-2</v>
       </c>
       <c r="CS24">
-        <f>ABS(CS15-CS16)</f>
+        <f t="shared" si="2"/>
         <v>1.6926054653999989E-2</v>
       </c>
       <c r="CT24">
-        <f>ABS(CT15-CT16)</f>
+        <f t="shared" si="2"/>
         <v>1.6576701352595979E-2</v>
       </c>
       <c r="CU24">
-        <f>ABS(CU15-CU16)</f>
+        <f t="shared" si="2"/>
         <v>9.5121351477769345E-3</v>
       </c>
       <c r="CV24">
-        <f>ABS(CV15-CV16)</f>
+        <f t="shared" si="2"/>
         <v>4.5733730066129796E-3</v>
       </c>
       <c r="CW24">
-        <f>ABS(CW15-CW16)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f xml:space="preserve"> AVERAGE(B24:Y24)</f>
+        <v>1.4250221218252648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>